<commit_message>
Ruter kan også være litt kortere enn T
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="14100" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation" r:id="rId1" sheetId="1"/>
-    <sheet name="One route" r:id="rId2" sheetId="3"/>
+    <sheet name="Simulation" sheetId="1" r:id="rId1"/>
+    <sheet name="One route" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'One route'!$A$2:$Y$2</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Simulation!$A$2:$AA$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$2:$Z$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -140,14 +140,13 @@
     <t>EXACT_METHOD</t>
   </si>
   <si>
-    <t>HEURISTIC_VERSION_1</t>
+    <t>Treshold length route</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,57 +191,60 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -259,10 +261,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -297,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -332,7 +334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -426,21 +428,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -457,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -509,89 +511,91 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="21.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="28" max="28" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:29" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="11" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
     </row>
-    <row customHeight="1" ht="48.75" r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -658,23 +662,26 @@
       <c r="V2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-0.25</v>
       </c>
@@ -741,199 +748,118 @@
       <c r="V3">
         <v>5</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>1.0324393939393939</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>1.0440121212121212</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>2.7272727272727275</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>11.2</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>11.106816242424236</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J4" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0.27276181818181816</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.2867509090909091</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.9090909090909092</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>11.823863127272721</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F5" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AA2"/>
+  <autoFilter ref="A2:AB2"/>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:V1"/>
+    <mergeCell ref="L1:W1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" style="1" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:28" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="14" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="10"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
       <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
     </row>
-    <row customHeight="1" ht="40.5" r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1000,19 +926,22 @@
       <c r="V2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="5"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="5"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-0.2</v>
       </c>
@@ -1079,29 +1008,29 @@
       <c r="V3">
         <v>2</v>
       </c>
-      <c r="W3">
+      <c r="X3" s="1">
         <v>0.19700000000000001</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>0.309</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>11.568199999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F4" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Y2"/>
+  <autoFilter ref="A2:Z2"/>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:V1"/>
-    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="X1:Z1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lager rute hvor bilen ikke gjør noe
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$2:$Z$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$9</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -141,13 +141,22 @@
   </si>
   <si>
     <t>Treshold length route</t>
+  </si>
+  <si>
+    <t>HEURISTIC_VERSION_1</t>
+  </si>
+  <si>
+    <t>HEURISTIC_VERSION_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -159,6 +168,13 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,6 +243,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -239,6 +258,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:W3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,65 +553,64 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="12.85546875" hidden="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.140625" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="21.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.140625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.42578125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.5703125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
       <c r="X1" s="12" t="s">
         <v>26</v>
       </c>
@@ -681,7 +702,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-0.25</v>
       </c>
@@ -748,27 +769,490 @@
       <c r="V3">
         <v>5</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="13">
         <v>1.0324393939393939</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="14">
         <v>1.0440121212121212</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="15">
         <v>2.7272727272727275</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="15">
         <v>11.2</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="15">
         <v>11.106816242424236</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F5" s="8"/>
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-0.25</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>-0.25</v>
+      </c>
+      <c r="D4">
+        <v>0.25</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.6</v>
+      </c>
+      <c r="I4">
+        <v>0.4</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+      <c r="P4">
+        <v>7</v>
+      </c>
+      <c r="Q4">
+        <v>9</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4">
+        <v>5</v>
+      </c>
+      <c r="X4" s="13">
+        <v>0.27875818181818179</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>0.29505818181818183</v>
+      </c>
+      <c r="Z4" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="15">
+        <v>10.6</v>
+      </c>
+      <c r="AB4" s="15">
+        <v>11.691497963636358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.25</v>
+      </c>
+      <c r="B5">
+        <v>0.25</v>
+      </c>
+      <c r="C5">
+        <v>-0.25</v>
+      </c>
+      <c r="D5">
+        <v>0.25</v>
+      </c>
+      <c r="E5">
+        <v>0.6</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+      <c r="H5">
+        <v>0.6</v>
+      </c>
+      <c r="I5">
+        <v>0.4</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>9</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5" s="13">
+        <v>9.0427272727272731E-2</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>0.10485272727272725</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>10.6</v>
+      </c>
+      <c r="AB5" s="15">
+        <v>11.657690290909084</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-0.25</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6">
+        <v>-0.25</v>
+      </c>
+      <c r="D6">
+        <v>0.25</v>
+      </c>
+      <c r="E6">
+        <v>0.6</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <v>0.6</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
+      <c r="Q6">
+        <v>9</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>5</v>
+      </c>
+      <c r="X6" s="13">
+        <v>4.5200000000000004E-2</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>6.1380000000000004E-2</v>
+      </c>
+      <c r="Z6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="15">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="15">
+        <v>12.278333333333325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-0.25</v>
+      </c>
+      <c r="B7">
+        <v>0.25</v>
+      </c>
+      <c r="C7">
+        <v>-0.25</v>
+      </c>
+      <c r="D7">
+        <v>0.25</v>
+      </c>
+      <c r="E7">
+        <v>0.6</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.6</v>
+      </c>
+      <c r="I7">
+        <v>0.4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7">
+        <v>11</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>7.6789473684210519E-2</v>
+      </c>
+      <c r="Y7">
+        <v>0.13589473684210529</v>
+      </c>
+      <c r="Z7" s="20">
+        <v>42.125382262996943</v>
+      </c>
+      <c r="AA7">
+        <v>38</v>
+      </c>
+      <c r="AB7">
+        <v>6.3464912280701773</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+      <c r="I8">
+        <v>0.4</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>18</v>
+      </c>
+      <c r="L8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="F9">
+        <v>0.3</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.6</v>
+      </c>
+      <c r="I9">
+        <v>0.4</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>18</v>
+      </c>
+      <c r="L9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0.6</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.6</v>
+      </c>
+      <c r="I10">
+        <v>0.4</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>18</v>
+      </c>
+      <c r="L10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="F11">
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>0.6</v>
+      </c>
+      <c r="I11">
+        <v>0.4</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>18</v>
+      </c>
+      <c r="L11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AB2"/>
+  <autoFilter ref="A2:AB9">
+    <filterColumn colId="17">
+      <filters>
+        <filter val="5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:I1"/>
@@ -811,7 +1295,7 @@
     <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="16.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -820,42 +1304,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
       <c r="W1" s="11"/>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
     </row>

</xml_diff>

<commit_message>
Printer resultat mellom hver kjøring
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView windowHeight="14100" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation" sheetId="1" r:id="rId1"/>
-    <sheet name="One route" sheetId="3" r:id="rId2"/>
+    <sheet name="Simulation" r:id="rId1" sheetId="1"/>
+    <sheet name="One route" r:id="rId2" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$2:$Z$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$9</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'One route'!$A$2:$Z$2</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Simulation!$A$2:$AB$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -137,13 +137,7 @@
     <t>Simulation stop time, min</t>
   </si>
   <si>
-    <t>EXACT_METHOD</t>
-  </si>
-  <si>
     <t>Treshold length route</t>
-  </si>
-  <si>
-    <t>HEURISTIC_VERSION_1</t>
   </si>
   <si>
     <t>HEURISTIC_VERSION_2</t>
@@ -207,64 +201,64 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -281,10 +275,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -319,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -354,7 +348,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -448,21 +442,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -479,7 +473,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -531,54 +525,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB13" sqref="A7:AB13"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="21.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22.42578125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.5703125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" hidden="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="10.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" hidden="true" width="14.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" hidden="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" hidden="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" hidden="true" width="12.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="12" width="21.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="13" width="22.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="15" width="15.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="14" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="14" width="17.5703125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -610,12 +604,12 @@
       <c r="U1" s="17"/>
       <c r="V1" s="17"/>
       <c r="W1" s="17"/>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="16" t="s">
         <v>26</v>
       </c>
       <c r="AC1" s="9"/>
     </row>
-    <row r="2" spans="1:29" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48.75" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -683,7 +677,7 @@
         <v>22</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>27</v>
@@ -701,530 +695,94 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-0.25</v>
-      </c>
-      <c r="B3">
-        <v>0.25</v>
-      </c>
-      <c r="C3">
-        <v>-0.25</v>
-      </c>
-      <c r="D3">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="1">
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.6</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>0.3</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>0.1</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>0.6</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>0.4</v>
       </c>
-      <c r="J3" s="1">
-        <v>5</v>
-      </c>
-      <c r="K3">
-        <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>37</v>
+      <c r="J3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>20</v>
-      </c>
-      <c r="P3">
-        <v>7</v>
-      </c>
-      <c r="Q3">
-        <v>9</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>5</v>
-      </c>
-      <c r="X3" s="13">
-        <v>1.0324393939393939</v>
-      </c>
-      <c r="Y3" s="14">
-        <v>1.0440121212121212</v>
-      </c>
-      <c r="Z3" s="15">
-        <v>2.7272727272727275</v>
-      </c>
-      <c r="AA3" s="15">
-        <v>11.2</v>
-      </c>
-      <c r="AB3" s="15">
-        <v>11.106816242424236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-0.25</v>
-      </c>
-      <c r="B4">
-        <v>0.25</v>
-      </c>
-      <c r="C4">
-        <v>-0.25</v>
-      </c>
-      <c r="D4">
-        <v>0.25</v>
-      </c>
-      <c r="E4">
-        <v>0.6</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-      <c r="G4">
-        <v>0.1</v>
-      </c>
-      <c r="H4">
-        <v>0.6</v>
-      </c>
-      <c r="I4">
-        <v>0.4</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>20</v>
-      </c>
-      <c r="P4">
-        <v>7</v>
-      </c>
-      <c r="Q4">
-        <v>9</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>2</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>5</v>
-      </c>
-      <c r="W4">
-        <v>5</v>
-      </c>
-      <c r="X4" s="13">
-        <v>0.27875818181818179</v>
-      </c>
-      <c r="Y4" s="14">
-        <v>0.29505818181818183</v>
-      </c>
-      <c r="Z4" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="15">
-        <v>10.6</v>
-      </c>
-      <c r="AB4" s="15">
-        <v>11.691497963636358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-0.25</v>
-      </c>
-      <c r="B5">
-        <v>0.25</v>
-      </c>
-      <c r="C5">
-        <v>-0.25</v>
-      </c>
-      <c r="D5">
-        <v>0.25</v>
-      </c>
-      <c r="E5">
-        <v>0.6</v>
-      </c>
-      <c r="F5">
-        <v>0.3</v>
-      </c>
-      <c r="G5">
-        <v>0.1</v>
-      </c>
-      <c r="H5">
-        <v>0.6</v>
-      </c>
-      <c r="I5">
-        <v>0.4</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>20</v>
-      </c>
-      <c r="P5">
-        <v>7</v>
-      </c>
-      <c r="Q5">
-        <v>9</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>2</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>5</v>
-      </c>
-      <c r="W5">
-        <v>5</v>
-      </c>
-      <c r="X5" s="13">
-        <v>9.0427272727272731E-2</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>0.10485272727272725</v>
-      </c>
-      <c r="Z5" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="15">
-        <v>10.6</v>
-      </c>
-      <c r="AB5" s="15">
-        <v>11.657690290909084</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-0.25</v>
-      </c>
-      <c r="B6">
-        <v>0.25</v>
-      </c>
-      <c r="C6">
-        <v>-0.25</v>
-      </c>
-      <c r="D6">
-        <v>0.25</v>
-      </c>
-      <c r="E6">
-        <v>0.6</v>
-      </c>
-      <c r="F6">
-        <v>0.3</v>
-      </c>
-      <c r="G6">
-        <v>0.1</v>
-      </c>
-      <c r="H6">
-        <v>0.6</v>
-      </c>
-      <c r="I6">
-        <v>0.4</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>20</v>
-      </c>
-      <c r="P6">
-        <v>7</v>
-      </c>
-      <c r="Q6">
-        <v>9</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>2</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>5</v>
-      </c>
-      <c r="W6">
-        <v>5</v>
-      </c>
-      <c r="X6" s="13">
-        <v>4.5200000000000004E-2</v>
-      </c>
-      <c r="Y6" s="14">
-        <v>6.1380000000000004E-2</v>
-      </c>
-      <c r="Z6" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="15">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="15">
-        <v>12.278333333333325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>0.6</v>
-      </c>
-      <c r="F7">
-        <v>0.3</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>0.6</v>
-      </c>
-      <c r="I7">
-        <v>0.4</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>18</v>
-      </c>
-      <c r="L7"/>
-      <c r="P7">
-        <v>7</v>
-      </c>
-      <c r="Q7">
-        <v>11</v>
-      </c>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>0.6</v>
-      </c>
-      <c r="F8">
-        <v>0.3</v>
-      </c>
-      <c r="G8">
-        <v>0.1</v>
-      </c>
-      <c r="H8">
-        <v>0.6</v>
-      </c>
-      <c r="I8">
-        <v>0.4</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>18</v>
-      </c>
-      <c r="L8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <v>0.6</v>
-      </c>
-      <c r="F9">
-        <v>0.3</v>
-      </c>
-      <c r="G9">
-        <v>0.1</v>
-      </c>
-      <c r="H9">
-        <v>0.6</v>
-      </c>
-      <c r="I9">
-        <v>0.4</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
-        <v>18</v>
-      </c>
-      <c r="L9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <v>0.6</v>
-      </c>
-      <c r="F10">
-        <v>0.3</v>
-      </c>
-      <c r="G10">
-        <v>0.1</v>
-      </c>
-      <c r="H10">
-        <v>0.6</v>
-      </c>
-      <c r="I10">
-        <v>0.4</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>18</v>
-      </c>
-      <c r="L10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <v>0.6</v>
-      </c>
-      <c r="F11">
-        <v>0.3</v>
-      </c>
-      <c r="G11">
-        <v>0.1</v>
-      </c>
-      <c r="H11">
-        <v>0.6</v>
-      </c>
-      <c r="I11">
-        <v>0.4</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11">
-        <v>18</v>
-      </c>
-      <c r="L11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <v>0.6</v>
-      </c>
-      <c r="F12">
-        <v>0.3</v>
-      </c>
-      <c r="G12">
-        <v>0.1</v>
-      </c>
-      <c r="H12">
-        <v>0.6</v>
-      </c>
-      <c r="I12">
-        <v>0.4</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12">
-        <v>18</v>
-      </c>
-      <c r="L12"/>
-      <c r="P12">
-        <v>7</v>
-      </c>
-      <c r="Q12">
-        <v>11</v>
-      </c>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
+      <c r="N3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.7760471610845295</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.7875765970072237</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>50.275881409689255</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>12.58442889158457</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AB9">
+  <autoFilter ref="A2:AB2">
     <filterColumn colId="17">
       <filters>
         <filter val="5"/>
@@ -1237,14 +795,14 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:W1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
@@ -1252,36 +810,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="12" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +879,7 @@
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
     </row>
-    <row r="2" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.5" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1389,7 +947,7 @@
         <v>22</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>27</v>
@@ -1492,7 +1050,7 @@
     <mergeCell ref="L1:V1"/>
     <mergeCell ref="X1:Z1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Klar til nattkjøring. Testing av criticality score
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -167,8 +167,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
@@ -237,7 +237,6 @@
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -253,6 +252,14 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -534,10 +541,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,47 +573,48 @@
     <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" style="12" width="21.28515625" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" style="13" width="22.42578125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="15" width="15.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="23" width="15.0" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="14" width="20.7109375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="14" width="17.5703125" collapsed="true"/>
     <col min="29" max="29" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="16" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="15" t="s">
         <v>26</v>
       </c>
+      <c r="Z1" s="20"/>
       <c r="AC1" s="9"/>
     </row>
     <row customHeight="1" ht="48.75" r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -685,7 +693,7 @@
       <c r="Y2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AA2" s="3" t="s">
@@ -695,39 +703,39 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>-0.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F3" t="n">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+      <c r="F3">
         <v>0.3</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0.1</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="H3">
+        <v>0.6</v>
+      </c>
+      <c r="I3">
         <v>0.4</v>
       </c>
-      <c r="J3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>18.0</v>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>18</v>
       </c>
       <c r="L3" t="s">
         <v>38</v>
@@ -735,50 +743,738 @@
       <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>7</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>15</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <v>0.77604716108452954</v>
+      </c>
+      <c r="Y3">
+        <v>0.78757659700722371</v>
+      </c>
+      <c r="Z3" s="22">
+        <v>50.275881409689255</v>
+      </c>
+      <c r="AA3">
+        <v>19.8</v>
+      </c>
+      <c r="AB3">
+        <v>12.584428891584571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>-0.1</v>
+      </c>
+      <c r="D4">
+        <v>0.9</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.6</v>
+      </c>
+      <c r="I4">
+        <v>0.4</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+      <c r="P4">
+        <v>7</v>
+      </c>
+      <c r="Q4">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>15</v>
+      </c>
+      <c r="W4">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>0.82238609478548574</v>
+      </c>
+      <c r="Y4">
+        <v>0.83516394022495855</v>
+      </c>
+      <c r="Z4" s="22">
+        <v>50.2713468605724</v>
+      </c>
+      <c r="AA4">
+        <v>19.333333333333332</v>
+      </c>
+      <c r="AB4">
+        <v>12.81881648931792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-0.2</v>
+      </c>
+      <c r="D5">
+        <v>0.8</v>
+      </c>
+      <c r="E5">
+        <v>0.6</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+      <c r="H5">
+        <v>0.6</v>
+      </c>
+      <c r="I5">
+        <v>0.4</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>11</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>15</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>0.82833611420954667</v>
+      </c>
+      <c r="Y5">
+        <v>0.83834166155947609</v>
+      </c>
+      <c r="Z5" s="22">
+        <v>50.273700019262975</v>
+      </c>
+      <c r="AA5">
+        <v>20.866666666666667</v>
+      </c>
+      <c r="AB5">
+        <v>11.918922905174659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+      <c r="E6">
+        <v>0.6</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <v>0.6</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
+      <c r="Q6">
+        <v>11</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>15</v>
+      </c>
+      <c r="W6">
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <v>0.93763379802001523</v>
+      </c>
+      <c r="Y6">
+        <v>0.94911775611827787</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>50.251089336635488</v>
+      </c>
+      <c r="AA6">
+        <v>23.266666666666666</v>
+      </c>
+      <c r="AB6">
+        <v>10.761223454400172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-0.4</v>
+      </c>
+      <c r="D7">
+        <v>0.6</v>
+      </c>
+      <c r="E7">
+        <v>0.6</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.6</v>
+      </c>
+      <c r="I7">
+        <v>0.4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7">
+        <v>11</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>15</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>1.1077126436262759</v>
+      </c>
+      <c r="Y7">
+        <v>1.1199387052389929</v>
+      </c>
+      <c r="Z7" s="22">
+        <v>50.244496220999032</v>
+      </c>
+      <c r="AA7">
+        <v>26.066666666666666</v>
+      </c>
+      <c r="AB7">
+        <v>9.4921988622969256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+      <c r="I8">
+        <v>0.4</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>11</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <v>15</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>1.3120421615237783</v>
+      </c>
+      <c r="Y8">
+        <v>1.325725838687192</v>
+      </c>
+      <c r="Z8" s="22">
+        <v>50.244748743535652</v>
+      </c>
+      <c r="AA8">
+        <v>28.666666666666668</v>
+      </c>
+      <c r="AB8">
+        <v>8.5707766304504727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>-0.6</v>
+      </c>
+      <c r="D9">
+        <v>0.4</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="F9">
+        <v>0.3</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.6</v>
+      </c>
+      <c r="I9">
+        <v>0.4</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>11</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>15</v>
+      </c>
+      <c r="W9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <v>1.5423999355250693</v>
+      </c>
+      <c r="Y9">
+        <v>1.5550176510251446</v>
+      </c>
+      <c r="Z9" s="22">
+        <v>50.239730735317188</v>
+      </c>
+      <c r="AA9">
+        <v>29.933333333333334</v>
+      </c>
+      <c r="AB9">
+        <v>8.1344702754030624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-0.7</v>
+      </c>
+      <c r="D10">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E10">
+        <v>0.6</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.6</v>
+      </c>
+      <c r="I10">
+        <v>0.4</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>20</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>11</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>3</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>1.9824286812481102</v>
+      </c>
+      <c r="Y10">
+        <v>1.9975900634567298</v>
+      </c>
+      <c r="Z10" s="22">
+        <v>50.233141709192338</v>
+      </c>
+      <c r="AA10">
+        <v>30.4</v>
+      </c>
+      <c r="AB10">
+        <v>8.0618021877846378</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.7999999999999999</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="n">
         <v>1.0</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O11" t="n">
         <v>20.0</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P11" t="n">
         <v>7.0</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q11" t="n">
         <v>11.0</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R11" t="n">
         <v>5.0</v>
       </c>
-      <c r="S3" t="n">
+      <c r="S11" t="n">
         <v>1.0</v>
       </c>
-      <c r="T3" t="n">
+      <c r="T11" t="n">
         <v>3.0</v>
       </c>
-      <c r="U3" t="n">
+      <c r="U11" t="n">
         <v>3.0</v>
       </c>
-      <c r="V3" t="n">
+      <c r="V11" t="n">
         <v>15.0</v>
       </c>
-      <c r="W3" t="n">
+      <c r="W11" t="n">
         <v>5.0</v>
       </c>
-      <c r="X3" t="n">
-        <v>0.7760471610845295</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.7875765970072237</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>50.275881409689255</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>19.8</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>12.58442889158457</v>
+      <c r="X11" t="n">
+        <v>2.8406041926214316</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2.8561671353973557</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>50.23138280802987</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>30.533333333333335</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>8.036007815254612</v>
       </c>
     </row>
   </sheetData>
@@ -795,6 +1491,18 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:W1"/>
   </mergeCells>
+  <conditionalFormatting sqref="Z3:Z1048576">
+    <cfRule priority="1" type="colorScale">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
@@ -840,42 +1548,42 @@
   </cols>
   <sheetData>
     <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
       <c r="W1" s="11"/>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
     </row>

</xml_diff>

<commit_message>
Klar til nattkjøring fortsettelse
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="14100" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation" r:id="rId1" sheetId="1"/>
-    <sheet name="One route" r:id="rId2" sheetId="3"/>
+    <sheet name="Simulation" sheetId="1" r:id="rId1"/>
+    <sheet name="One route" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'One route'!$A$2:$Z$2</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Simulation!$A$2:$AB$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$2:$Z$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -201,71 +201,71 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -282,10 +282,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -320,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -355,7 +355,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -449,21 +449,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -480,7 +480,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -532,92 +532,92 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" hidden="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="10.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" hidden="true" width="14.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" hidden="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" hidden="true" width="12.85546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="12" width="21.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="13" width="22.42578125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="23" width="15.0" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="14" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="14" width="17.5703125" collapsed="true"/>
-    <col min="29" max="29" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="12.85546875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.28515625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15" style="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17" t="s">
+    <row r="1" spans="1:29" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
       <c r="X1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="20"/>
+      <c r="Z1" s="16"/>
       <c r="AC1" s="9"/>
     </row>
-    <row customHeight="1" ht="48.75" r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="Y2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="Z2" s="17" t="s">
         <v>29</v>
       </c>
       <c r="AA2" s="3" t="s">
@@ -779,7 +779,7 @@
       <c r="Y3">
         <v>0.78757659700722371</v>
       </c>
-      <c r="Z3" s="22">
+      <c r="Z3" s="18">
         <v>50.275881409689255</v>
       </c>
       <c r="AA3">
@@ -865,7 +865,7 @@
       <c r="Y4">
         <v>0.83516394022495855</v>
       </c>
-      <c r="Z4" s="22">
+      <c r="Z4" s="18">
         <v>50.2713468605724</v>
       </c>
       <c r="AA4">
@@ -951,7 +951,7 @@
       <c r="Y5">
         <v>0.83834166155947609</v>
       </c>
-      <c r="Z5" s="22">
+      <c r="Z5" s="18">
         <v>50.273700019262975</v>
       </c>
       <c r="AA5">
@@ -1037,7 +1037,7 @@
       <c r="Y6">
         <v>0.94911775611827787</v>
       </c>
-      <c r="Z6" s="22">
+      <c r="Z6" s="18">
         <v>50.251089336635488</v>
       </c>
       <c r="AA6">
@@ -1123,7 +1123,7 @@
       <c r="Y7">
         <v>1.1199387052389929</v>
       </c>
-      <c r="Z7" s="22">
+      <c r="Z7" s="18">
         <v>50.244496220999032</v>
       </c>
       <c r="AA7">
@@ -1209,7 +1209,7 @@
       <c r="Y8">
         <v>1.325725838687192</v>
       </c>
-      <c r="Z8" s="22">
+      <c r="Z8" s="18">
         <v>50.244748743535652</v>
       </c>
       <c r="AA8">
@@ -1295,7 +1295,7 @@
       <c r="Y9">
         <v>1.5550176510251446</v>
       </c>
-      <c r="Z9" s="22">
+      <c r="Z9" s="18">
         <v>50.239730735317188</v>
       </c>
       <c r="AA9">
@@ -1381,7 +1381,7 @@
       <c r="Y10">
         <v>1.9975900634567298</v>
       </c>
-      <c r="Z10" s="22">
+      <c r="Z10" s="18">
         <v>50.233141709192338</v>
       </c>
       <c r="AA10">
@@ -1391,39 +1391,39 @@
         <v>8.0618021877846378</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>-0.0</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-0.7999999999999999</v>
-      </c>
-      <c r="D11" t="n">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-0.79999999999999993</v>
+      </c>
+      <c r="D11">
         <v>0.20000000000000007</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="F11">
         <v>0.3</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>0.1</v>
       </c>
-      <c r="H11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I11" t="n">
+      <c r="H11">
+        <v>0.6</v>
+      </c>
+      <c r="I11">
         <v>0.4</v>
       </c>
-      <c r="J11" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>18.0</v>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>18</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
@@ -1431,50 +1431,308 @@
       <c r="M11" t="s">
         <v>34</v>
       </c>
-      <c r="N11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="X11" t="n">
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>20</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>11</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11">
+        <v>15</v>
+      </c>
+      <c r="W11">
+        <v>5</v>
+      </c>
+      <c r="X11">
         <v>2.8406041926214316</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="Y11">
         <v>2.8561671353973557</v>
       </c>
-      <c r="Z11" t="n">
-        <v>50.23138280802987</v>
-      </c>
-      <c r="AA11" t="n">
+      <c r="Z11">
+        <v>50.231382808029871</v>
+      </c>
+      <c r="AA11">
         <v>30.533333333333335</v>
       </c>
-      <c r="AB11" t="n">
-        <v>8.036007815254612</v>
+      <c r="AB11">
+        <v>8.0360078152546119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="D12">
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="E12">
+        <v>0.6</v>
+      </c>
+      <c r="F12">
+        <v>0.3</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0.6</v>
+      </c>
+      <c r="I12">
+        <v>0.4</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>20</v>
+      </c>
+      <c r="P12">
+        <v>7</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>5</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <v>15</v>
+      </c>
+      <c r="W12">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>3.8678629146118579</v>
+      </c>
+      <c r="Y12">
+        <v>3.8918107891778635</v>
+      </c>
+      <c r="Z12">
+        <v>50.231950857711084</v>
+      </c>
+      <c r="AA12">
+        <v>28.733333333333334</v>
+      </c>
+      <c r="AB12">
+        <v>8.5134273967478027</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-0.99999999999999989</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>0.3</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>0.6</v>
+      </c>
+      <c r="I13">
+        <v>0.4</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>20</v>
+      </c>
+      <c r="P13">
+        <v>7</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>3</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <v>15</v>
+      </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
+      <c r="X13">
+        <v>4.3783958109319006</v>
+      </c>
+      <c r="Y13">
+        <v>4.401511680514826</v>
+      </c>
+      <c r="Z13">
+        <v>50.242622762003911</v>
+      </c>
+      <c r="AA13">
+        <v>31.333333333333332</v>
+      </c>
+      <c r="AB13">
+        <v>7.7750928836836097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.9</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="F14">
+        <v>0.3</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.6</v>
+      </c>
+      <c r="I14">
+        <v>0.4</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>20</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>5</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>15</v>
+      </c>
+      <c r="W14">
+        <v>5</v>
+      </c>
+      <c r="X14">
+        <v>0.7990273316982297</v>
+      </c>
+      <c r="Y14">
+        <v>0.80891343188631126</v>
+      </c>
+      <c r="Z14">
+        <v>50.275755849011354</v>
+      </c>
+      <c r="AA14">
+        <v>20.066666666666666</v>
+      </c>
+      <c r="AB14">
+        <v>12.343588938923956</v>
       </c>
     </row>
   </sheetData>
@@ -1492,7 +1750,7 @@
     <mergeCell ref="L1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="Z3:Z1048576">
-    <cfRule priority="1" type="colorScale">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1503,14 +1761,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
@@ -1518,76 +1776,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" style="1" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17" t="s">
+    <row r="1" spans="1:28" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
       <c r="W1" s="11"/>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
     </row>
-    <row customHeight="1" ht="40.5" r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1758,7 +2016,7 @@
     <mergeCell ref="L1:V1"/>
     <mergeCell ref="X1:Z1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Endrer objektivverdi på heuristikk 3 slik at den er lik som versjon 1 og 2
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -1510,7 +1510,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
@@ -1749,6 +1749,1846 @@
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F4" s="8"/>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.248</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>605.876</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.289</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>605.876</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1.593</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.948</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>1.014</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.962</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>1.025</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>605.876</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.282</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.339</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>593.781</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.243</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>594.449</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>593.781</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.243</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>593.781</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>593.781</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1.054</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>593.781</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.281</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>601.562</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.359</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>601.562</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>601.562</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.234</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>601.562</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>601.562</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.369</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>554.138</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.219</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.281</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J25" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.943</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M26" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>1.068</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J27" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.948</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>1.011</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>546.357</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:Z2"/>
   <mergeCells count="5">

</xml_diff>

<commit_message>
fikser pricing problem (marte)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="13215"/>
+    <workbookView windowHeight="13215" windowWidth="28215" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation" sheetId="1" r:id="rId1"/>
-    <sheet name="One route" sheetId="3" r:id="rId2"/>
+    <sheet name="Simulation" r:id="rId1" sheetId="1"/>
+    <sheet name="One route" r:id="rId2" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$2:$X$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$2:$AB$297</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'One route'!$A$2:$X$2</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Simulation!$A$2:$AB$297</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="42">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -210,73 +210,73 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -312,11 +312,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -352,7 +352,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln cap="rnd" w="28575">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1261,7 +1261,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1273,11 +1273,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1308,7 +1308,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -1332,11 +1332,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1371,7 +1371,7 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
       <a:solidFill>
         <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
@@ -1394,7 +1394,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1957,7 +1957,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1996,10 +1996,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2034,7 +2034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2069,7 +2069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2163,21 +2163,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2194,7 +2194,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2246,53 +2246,53 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC297"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
       <selection activeCell="Y299" sqref="Y299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="21.28515625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" hidden="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="10.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" hidden="true" width="14.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" hidden="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" hidden="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" hidden="true" width="12.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="12" width="21.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="13" width="22.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="19" width="15.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="14" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="14" width="17.5703125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2330,7 @@
       <c r="Z1" s="16"/>
       <c r="AC1" s="9"/>
     </row>
-    <row r="2" spans="1:29" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48.75" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>10.908975454874838</v>
       </c>
     </row>
-    <row r="61" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>0</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>8.884604550354565</v>
       </c>
     </row>
-    <row r="68" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="68" s="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
         <v>0</v>
       </c>
@@ -27228,7 +27228,7 @@
     <mergeCell ref="L1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="Z292:Z1048576 Z248:Z249 Z3:Z193 Z195:Z197 Z199:Z200 Z202 Z204:Z221 Z223:Z245 Z251 Z253:Z266 Z268:Z288">
-    <cfRule type="colorScale" priority="23">
+    <cfRule priority="23" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -27240,7 +27240,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z292:Z1048576 Z248:Z249 Z3:Z202 Z204:Z221 Z223:Z245 Z251 Z253:Z266 Z268:Z288">
-    <cfRule type="colorScale" priority="33">
+    <cfRule priority="33" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -27252,7 +27252,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z292:Z1048576 Z3:Z246 Z248:Z249 Z251 Z253:Z266 Z268:Z288">
-    <cfRule type="colorScale" priority="40">
+    <cfRule priority="40" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -27264,7 +27264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:Z288">
-    <cfRule type="colorScale" priority="1">
+    <cfRule priority="1" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -27275,15 +27275,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z296"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA336"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="X296" sqref="X11:X296"/>
@@ -27291,35 +27291,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="0" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" hidden="true" style="1" width="0.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" hidden="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" hidden="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" hidden="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="39.75" r="1" s="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -27357,7 +27357,7 @@
       <c r="Y1" s="10"/>
       <c r="Z1" s="10"/>
     </row>
-    <row r="2" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="57" r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -49053,6 +49053,2759 @@
       </c>
       <c r="X296">
         <v>551.88900000000001</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C297" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="D297" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E297" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F297" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G297" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H297" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I297" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L297" t="s">
+        <v>41</v>
+      </c>
+      <c r="M297" t="s">
+        <v>34</v>
+      </c>
+      <c r="N297" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O297" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P297" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R297" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S297" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T297" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W297" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X297" t="n">
+        <v>1.587</v>
+      </c>
+      <c r="Y297" t="n">
+        <v>1.657</v>
+      </c>
+      <c r="Z297" t="n">
+        <v>544.965</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C298" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="D298" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E298" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F298" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G298" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H298" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I298" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L298" t="s">
+        <v>41</v>
+      </c>
+      <c r="M298" t="s">
+        <v>34</v>
+      </c>
+      <c r="N298" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O298" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P298" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R298" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S298" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T298" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W298" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X298" t="n">
+        <v>1.708</v>
+      </c>
+      <c r="Y298" t="n">
+        <v>1.769</v>
+      </c>
+      <c r="Z298" t="n">
+        <v>544.965</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C299" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="D299" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E299" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F299" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G299" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I299" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L299" t="s">
+        <v>41</v>
+      </c>
+      <c r="M299" t="s">
+        <v>34</v>
+      </c>
+      <c r="N299" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O299" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P299" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R299" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S299" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T299" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W299" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X299" t="n">
+        <v>1.217</v>
+      </c>
+      <c r="Y299" t="n">
+        <v>1.224</v>
+      </c>
+      <c r="Z299" t="n">
+        <v>544.965</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B300" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C300" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="D300" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E300" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F300" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H300" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I300" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L300" t="s">
+        <v>41</v>
+      </c>
+      <c r="M300" t="s">
+        <v>34</v>
+      </c>
+      <c r="N300" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O300" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P300" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R300" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S300" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T300" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W300" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X300" t="n">
+        <v>1.545</v>
+      </c>
+      <c r="Y300" t="n">
+        <v>1.603</v>
+      </c>
+      <c r="Z300" t="n">
+        <v>544.965</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B301" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C301" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D301" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E301" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G301" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H301" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I301" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L301" t="s">
+        <v>41</v>
+      </c>
+      <c r="M301" t="s">
+        <v>34</v>
+      </c>
+      <c r="N301" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O301" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P301" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R301" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S301" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T301" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W301" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X301" t="n">
+        <v>2.508</v>
+      </c>
+      <c r="Y301" t="n">
+        <v>2.575</v>
+      </c>
+      <c r="Z301" t="n">
+        <v>544.679</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B302" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C302" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D302" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E302" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G302" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H302" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I302" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L302" t="s">
+        <v>41</v>
+      </c>
+      <c r="M302" t="s">
+        <v>34</v>
+      </c>
+      <c r="N302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O302" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P302" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R302" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T302" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W302" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X302" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>1.472</v>
+      </c>
+      <c r="Z302" t="n">
+        <v>544.577</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B303" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C303" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D303" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E303" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F303" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G303" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H303" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I303" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L303" t="s">
+        <v>41</v>
+      </c>
+      <c r="M303" t="s">
+        <v>34</v>
+      </c>
+      <c r="N303" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O303" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P303" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R303" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S303" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T303" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="W303" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X303" t="n">
+        <v>31.834</v>
+      </c>
+      <c r="Y303" t="n">
+        <v>32.025</v>
+      </c>
+      <c r="Z303" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B304" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C304" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D304" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E304" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F304" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G304" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H304" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I304" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L304" t="s">
+        <v>41</v>
+      </c>
+      <c r="M304" t="s">
+        <v>34</v>
+      </c>
+      <c r="N304" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O304" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P304" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R304" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S304" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T304" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W304" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X304" t="n">
+        <v>1.508</v>
+      </c>
+      <c r="Y304" t="n">
+        <v>1.583</v>
+      </c>
+      <c r="Z304" t="n">
+        <v>544.679</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B305" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C305" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D305" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E305" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F305" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G305" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H305" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I305" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L305" t="s">
+        <v>41</v>
+      </c>
+      <c r="M305" t="s">
+        <v>34</v>
+      </c>
+      <c r="N305" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O305" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P305" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R305" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S305" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T305" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W305" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X305" t="n">
+        <v>2.614</v>
+      </c>
+      <c r="Y305" t="n">
+        <v>2.708</v>
+      </c>
+      <c r="Z305" t="n">
+        <v>544.679</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B306" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C306" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D306" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E306" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F306" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G306" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H306" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I306" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L306" t="s">
+        <v>41</v>
+      </c>
+      <c r="M306" t="s">
+        <v>34</v>
+      </c>
+      <c r="N306" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O306" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P306" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R306" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S306" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T306" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W306" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X306" t="n">
+        <v>4.022</v>
+      </c>
+      <c r="Y306" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Z306" t="n">
+        <v>544.679</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B307" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C307" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D307" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E307" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F307" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G307" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H307" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I307" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L307" t="s">
+        <v>41</v>
+      </c>
+      <c r="M307" t="s">
+        <v>34</v>
+      </c>
+      <c r="N307" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O307" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P307" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R307" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S307" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T307" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W307" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X307" t="n">
+        <v>1.491</v>
+      </c>
+      <c r="Y307" t="n">
+        <v>1.553</v>
+      </c>
+      <c r="Z307" t="n">
+        <v>543.81</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B308" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C308" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D308" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E308" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F308" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G308" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H308" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I308" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L308" t="s">
+        <v>41</v>
+      </c>
+      <c r="M308" t="s">
+        <v>34</v>
+      </c>
+      <c r="N308" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O308" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P308" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R308" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S308" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T308" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W308" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X308" t="n">
+        <v>1.482</v>
+      </c>
+      <c r="Y308" t="n">
+        <v>1.536</v>
+      </c>
+      <c r="Z308" t="n">
+        <v>544.679</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B309" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C309" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E309" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F309" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G309" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H309" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I309" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L309" t="s">
+        <v>41</v>
+      </c>
+      <c r="M309" t="s">
+        <v>34</v>
+      </c>
+      <c r="N309" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O309" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P309" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R309" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S309" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T309" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W309" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X309" t="n">
+        <v>3.968</v>
+      </c>
+      <c r="Y309" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="Z309" t="n">
+        <v>542.708</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B310" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C310" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D310" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E310" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F310" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G310" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H310" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I310" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L310" t="s">
+        <v>41</v>
+      </c>
+      <c r="M310" t="s">
+        <v>34</v>
+      </c>
+      <c r="N310" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O310" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P310" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R310" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S310" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T310" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="W310" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X310" t="n">
+        <v>5.516</v>
+      </c>
+      <c r="Y310" t="n">
+        <v>5.626</v>
+      </c>
+      <c r="Z310" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B311" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C311" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D311" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E311" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F311" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G311" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H311" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I311" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J311" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K311" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L311" t="s">
+        <v>37</v>
+      </c>
+      <c r="M311" t="s">
+        <v>34</v>
+      </c>
+      <c r="N311" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O311" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P311" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R311" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S311" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T311" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U311" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W311" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X311" t="n">
+        <v>1.781</v>
+      </c>
+      <c r="Y311" t="n">
+        <v>1.849</v>
+      </c>
+      <c r="Z311" t="n">
+        <v>544.909</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B312" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C312" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D312" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E312" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F312" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G312" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H312" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I312" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J312" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K312" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L312" t="s">
+        <v>37</v>
+      </c>
+      <c r="M312" t="s">
+        <v>34</v>
+      </c>
+      <c r="N312" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O312" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P312" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R312" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S312" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T312" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U312" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W312" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X312" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="Y312" t="n">
+        <v>1.812</v>
+      </c>
+      <c r="Z312" t="n">
+        <v>543.337</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B313" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C313" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D313" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E313" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F313" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G313" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H313" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I313" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J313" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K313" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L313" t="s">
+        <v>37</v>
+      </c>
+      <c r="M313" t="s">
+        <v>34</v>
+      </c>
+      <c r="N313" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O313" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P313" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R313" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S313" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T313" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U313" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W313" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X313" t="n">
+        <v>3.531</v>
+      </c>
+      <c r="Y313" t="n">
+        <v>3.609</v>
+      </c>
+      <c r="Z313" t="n">
+        <v>544.909</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B314" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C314" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D314" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E314" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F314" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G314" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H314" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I314" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J314" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K314" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L314" t="s">
+        <v>37</v>
+      </c>
+      <c r="M314" t="s">
+        <v>34</v>
+      </c>
+      <c r="N314" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O314" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P314" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R314" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S314" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T314" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U314" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W314" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X314" t="n">
+        <v>3.498</v>
+      </c>
+      <c r="Y314" t="n">
+        <v>3.561</v>
+      </c>
+      <c r="Z314" t="n">
+        <v>543.622</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B315" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C315" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D315" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E315" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F315" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G315" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H315" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I315" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J315" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K315" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L315" t="s">
+        <v>37</v>
+      </c>
+      <c r="M315" t="s">
+        <v>34</v>
+      </c>
+      <c r="N315" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O315" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P315" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R315" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S315" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T315" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U315" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W315" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X315" t="n">
+        <v>1.788</v>
+      </c>
+      <c r="Y315" t="n">
+        <v>1.851</v>
+      </c>
+      <c r="Z315" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B316" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C316" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D316" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E316" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F316" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G316" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H316" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I316" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J316" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K316" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L316" t="s">
+        <v>37</v>
+      </c>
+      <c r="M316" t="s">
+        <v>34</v>
+      </c>
+      <c r="N316" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O316" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P316" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R316" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S316" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T316" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U316" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W316" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X316" t="n">
+        <v>6.878</v>
+      </c>
+      <c r="Y316" t="n">
+        <v>6.971</v>
+      </c>
+      <c r="Z316" t="n">
+        <v>544.909</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B317" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C317" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D317" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E317" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F317" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G317" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H317" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I317" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J317" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K317" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L317" t="s">
+        <v>37</v>
+      </c>
+      <c r="M317" t="s">
+        <v>34</v>
+      </c>
+      <c r="N317" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O317" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P317" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R317" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S317" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T317" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U317" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W317" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X317" t="n">
+        <v>1.788</v>
+      </c>
+      <c r="Y317" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="Z317" t="n">
+        <v>543.436</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B318" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C318" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D318" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E318" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F318" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G318" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H318" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I318" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J318" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K318" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L318" t="s">
+        <v>37</v>
+      </c>
+      <c r="M318" t="s">
+        <v>34</v>
+      </c>
+      <c r="N318" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O318" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P318" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R318" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S318" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T318" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U318" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W318" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X318" t="n">
+        <v>6.859</v>
+      </c>
+      <c r="Y318" t="n">
+        <v>6.937</v>
+      </c>
+      <c r="Z318" t="n">
+        <v>543.242</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B319" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C319" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D319" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E319" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F319" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G319" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H319" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I319" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J319" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K319" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L319" t="s">
+        <v>37</v>
+      </c>
+      <c r="M319" t="s">
+        <v>34</v>
+      </c>
+      <c r="N319" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O319" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P319" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R319" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S319" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T319" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="U319" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W319" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X319" t="n">
+        <v>9.799</v>
+      </c>
+      <c r="Y319" t="n">
+        <v>9.91</v>
+      </c>
+      <c r="Z319" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B320" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C320" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D320" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E320" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F320" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G320" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H320" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I320" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J320" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K320" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L320" t="s">
+        <v>37</v>
+      </c>
+      <c r="M320" t="s">
+        <v>34</v>
+      </c>
+      <c r="N320" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O320" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P320" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R320" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S320" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T320" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="U320" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W320" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X320" t="n">
+        <v>15.217</v>
+      </c>
+      <c r="Y320" t="n">
+        <v>15.375</v>
+      </c>
+      <c r="Z320" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B321" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C321" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D321" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E321" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F321" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G321" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H321" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I321" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J321" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K321" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L321" t="s">
+        <v>37</v>
+      </c>
+      <c r="M321" t="s">
+        <v>34</v>
+      </c>
+      <c r="N321" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O321" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P321" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R321" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S321" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T321" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U321" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W321" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X321" t="n">
+        <v>6.856</v>
+      </c>
+      <c r="Y321" t="n">
+        <v>6.937</v>
+      </c>
+      <c r="Z321" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B322" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C322" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D322" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E322" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F322" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G322" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H322" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I322" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J322" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K322" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L322" t="s">
+        <v>37</v>
+      </c>
+      <c r="M322" t="s">
+        <v>34</v>
+      </c>
+      <c r="N322" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O322" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P322" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R322" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S322" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T322" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="U322" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W322" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X322" t="n">
+        <v>14.972</v>
+      </c>
+      <c r="Y322" t="n">
+        <v>15.124</v>
+      </c>
+      <c r="Z322" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B323" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C323" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D323" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E323" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F323" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G323" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H323" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I323" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J323" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K323" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L323" t="s">
+        <v>37</v>
+      </c>
+      <c r="M323" t="s">
+        <v>34</v>
+      </c>
+      <c r="N323" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O323" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P323" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R323" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S323" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T323" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="U323" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W323" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X323" t="n">
+        <v>9.613</v>
+      </c>
+      <c r="Y323" t="n">
+        <v>9.707</v>
+      </c>
+      <c r="Z323" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B324" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C324" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D324" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E324" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F324" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G324" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H324" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I324" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L324" t="s">
+        <v>41</v>
+      </c>
+      <c r="M324" t="s">
+        <v>34</v>
+      </c>
+      <c r="N324" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O324" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P324" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R324" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S324" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T324" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W324" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X324" t="n">
+        <v>4.303</v>
+      </c>
+      <c r="Y324" t="n">
+        <v>4.389</v>
+      </c>
+      <c r="Z324" t="n">
+        <v>543.261</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B325" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C325" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D325" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E325" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F325" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G325" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H325" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I325" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L325" t="s">
+        <v>41</v>
+      </c>
+      <c r="M325" t="s">
+        <v>34</v>
+      </c>
+      <c r="N325" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O325" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P325" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R325" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S325" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T325" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="W325" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X325" t="n">
+        <v>5.521</v>
+      </c>
+      <c r="Y325" t="n">
+        <v>5.599</v>
+      </c>
+      <c r="Z325" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B326" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C326" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D326" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E326" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F326" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G326" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H326" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I326" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L326" t="s">
+        <v>41</v>
+      </c>
+      <c r="M326" t="s">
+        <v>34</v>
+      </c>
+      <c r="N326" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O326" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P326" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R326" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S326" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T326" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W326" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X326" t="n">
+        <v>3.855</v>
+      </c>
+      <c r="Y326" t="n">
+        <v>3.952</v>
+      </c>
+      <c r="Z326" t="n">
+        <v>543.85</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B327" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C327" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D327" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E327" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F327" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G327" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H327" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I327" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L327" t="s">
+        <v>41</v>
+      </c>
+      <c r="M327" t="s">
+        <v>34</v>
+      </c>
+      <c r="N327" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O327" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P327" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R327" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S327" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T327" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="W327" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X327" t="n">
+        <v>5.491</v>
+      </c>
+      <c r="Y327" t="n">
+        <v>5.585</v>
+      </c>
+      <c r="Z327" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B328" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C328" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D328" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E328" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F328" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G328" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H328" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I328" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L328" t="s">
+        <v>41</v>
+      </c>
+      <c r="M328" t="s">
+        <v>34</v>
+      </c>
+      <c r="N328" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O328" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P328" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R328" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S328" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T328" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W328" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X328" t="n">
+        <v>3.992</v>
+      </c>
+      <c r="Y328" t="n">
+        <v>4.054</v>
+      </c>
+      <c r="Z328" t="n">
+        <v>542.593</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B329" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C329" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D329" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E329" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F329" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G329" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H329" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I329" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L329" t="s">
+        <v>41</v>
+      </c>
+      <c r="M329" t="s">
+        <v>34</v>
+      </c>
+      <c r="N329" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O329" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P329" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R329" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S329" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T329" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="W329" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X329" t="n">
+        <v>9.416</v>
+      </c>
+      <c r="Y329" t="n">
+        <v>9.556</v>
+      </c>
+      <c r="Z329" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B330" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C330" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D330" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E330" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F330" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G330" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H330" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I330" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L330" t="s">
+        <v>41</v>
+      </c>
+      <c r="M330" t="s">
+        <v>34</v>
+      </c>
+      <c r="N330" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O330" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P330" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R330" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S330" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T330" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="W330" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X330" t="n">
+        <v>9.166</v>
+      </c>
+      <c r="Y330" t="n">
+        <v>9.307</v>
+      </c>
+      <c r="Z330" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B331" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C331" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D331" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E331" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F331" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G331" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H331" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I331" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L331" t="s">
+        <v>41</v>
+      </c>
+      <c r="M331" t="s">
+        <v>34</v>
+      </c>
+      <c r="N331" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O331" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P331" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R331" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S331" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T331" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="W331" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X331" t="n">
+        <v>9.51</v>
+      </c>
+      <c r="Y331" t="n">
+        <v>9.635</v>
+      </c>
+      <c r="Z331" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B332" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C332" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D332" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E332" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F332" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G332" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H332" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I332" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L332" t="s">
+        <v>41</v>
+      </c>
+      <c r="M332" t="s">
+        <v>34</v>
+      </c>
+      <c r="N332" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O332" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P332" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R332" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S332" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T332" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="W332" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X332" t="n">
+        <v>9.354</v>
+      </c>
+      <c r="Y332" t="n">
+        <v>9.47</v>
+      </c>
+      <c r="Z332" t="n">
+        <v>542.823</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B333" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C333" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D333" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E333" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F333" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G333" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H333" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I333" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J333" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K333" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L333" t="s">
+        <v>37</v>
+      </c>
+      <c r="M333" t="s">
+        <v>34</v>
+      </c>
+      <c r="N333" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O333" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P333" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R333" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S333" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T333" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U333" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W333" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X333" t="n">
+        <v>6.897</v>
+      </c>
+      <c r="Y333" t="n">
+        <v>6.979</v>
+      </c>
+      <c r="Z333" t="n">
+        <v>543.353</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B334" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C334" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D334" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E334" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F334" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G334" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H334" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I334" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J334" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K334" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L334" t="s">
+        <v>37</v>
+      </c>
+      <c r="M334" t="s">
+        <v>34</v>
+      </c>
+      <c r="N334" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O334" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P334" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R334" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S334" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T334" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U334" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W334" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X334" t="n">
+        <v>6.724</v>
+      </c>
+      <c r="Y334" t="n">
+        <v>6.818</v>
+      </c>
+      <c r="Z334" t="n">
+        <v>543.337</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B335" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C335" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D335" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E335" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F335" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G335" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H335" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I335" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J335" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K335" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L335" t="s">
+        <v>37</v>
+      </c>
+      <c r="M335" t="s">
+        <v>34</v>
+      </c>
+      <c r="N335" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O335" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P335" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R335" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S335" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T335" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="U335" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W335" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X335" t="n">
+        <v>16.856</v>
+      </c>
+      <c r="Y335" t="n">
+        <v>16.997</v>
+      </c>
+      <c r="Z335" t="n">
+        <v>543.258</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>-0.0</v>
+      </c>
+      <c r="B336" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C336" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D336" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E336" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F336" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G336" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H336" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I336" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J336" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K336" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L336" t="s">
+        <v>37</v>
+      </c>
+      <c r="M336" t="s">
+        <v>34</v>
+      </c>
+      <c r="N336" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O336" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P336" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="R336" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S336" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T336" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="U336" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W336" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X336" t="n">
+        <v>6.764</v>
+      </c>
+      <c r="Y336" t="n">
+        <v>6.857</v>
+      </c>
+      <c r="Z336" t="n">
+        <v>543.218</v>
       </c>
     </row>
   </sheetData>
@@ -49065,7 +51818,7 @@
     <mergeCell ref="V1:X1"/>
   </mergeCells>
   <conditionalFormatting sqref="X11:X296">
-    <cfRule type="colorScale" priority="1">
+    <cfRule priority="1" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -49076,7 +51829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gjør currentSolution litt dårligere: tar bort regret, velger blant top 5, egne vekter
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file.stud.iot.ntnu.no\Home\kristi6\Documents\masteroppgave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="44">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>HEURISTIC_VERSION_1</t>
+  </si>
+  <si>
+    <t>CURRENT_SOLUTION_IN_OSLO</t>
+  </si>
+  <si>
+    <t>best evekter fra over</t>
   </si>
 </sst>
 </file>
@@ -2254,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD297"/>
+  <dimension ref="A1:AD301"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <selection activeCell="Y299" sqref="Y299"/>
+      <selection activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27014,7 +27020,7 @@
         <v>14.411938074446738</v>
       </c>
     </row>
-    <row r="289" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E289">
         <v>0.6</v>
       </c>
@@ -27049,7 +27055,7 @@
       <c r="AA289"/>
       <c r="AB289"/>
     </row>
-    <row r="290" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E290">
         <v>0.6</v>
       </c>
@@ -27084,7 +27090,7 @@
       <c r="AA290"/>
       <c r="AB290"/>
     </row>
-    <row r="291" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Y291" s="13" t="s">
         <v>38</v>
       </c>
@@ -27093,7 +27099,7 @@
         <v>50.22111857059717</v>
       </c>
     </row>
-    <row r="292" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Y292" s="13" t="s">
         <v>39</v>
       </c>
@@ -27102,7 +27108,7 @@
         <v>50.33646608706686</v>
       </c>
     </row>
-    <row r="293" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B293">
         <v>0.3</v>
       </c>
@@ -27179,7 +27185,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="294" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E294"/>
       <c r="J294"/>
       <c r="L294"/>
@@ -27189,7 +27195,7 @@
       <c r="AA294"/>
       <c r="AB294"/>
     </row>
-    <row r="295" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E295"/>
       <c r="J295"/>
       <c r="L295"/>
@@ -27199,7 +27205,7 @@
       <c r="AA295"/>
       <c r="AB295"/>
     </row>
-    <row r="296" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E296"/>
       <c r="J296"/>
       <c r="L296"/>
@@ -27209,7 +27215,7 @@
       <c r="AA296"/>
       <c r="AB296"/>
     </row>
-    <row r="297" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E297"/>
       <c r="J297"/>
       <c r="L297"/>
@@ -27218,6 +27224,269 @@
       <c r="Z297"/>
       <c r="AA297"/>
       <c r="AB297"/>
+    </row>
+    <row r="298" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>43</v>
+      </c>
+      <c r="E298">
+        <v>0.6</v>
+      </c>
+      <c r="F298">
+        <v>0.3</v>
+      </c>
+      <c r="G298">
+        <v>0.1</v>
+      </c>
+      <c r="H298">
+        <v>0.6</v>
+      </c>
+      <c r="I298">
+        <v>0.4</v>
+      </c>
+      <c r="J298">
+        <v>5</v>
+      </c>
+      <c r="K298">
+        <v>18</v>
+      </c>
+      <c r="L298" t="s">
+        <v>42</v>
+      </c>
+      <c r="M298" t="s">
+        <v>34</v>
+      </c>
+      <c r="N298">
+        <v>1</v>
+      </c>
+      <c r="O298">
+        <v>20</v>
+      </c>
+      <c r="P298">
+        <v>7</v>
+      </c>
+      <c r="Q298">
+        <v>11</v>
+      </c>
+      <c r="R298">
+        <v>5</v>
+      </c>
+      <c r="S298">
+        <v>2</v>
+      </c>
+      <c r="V298">
+        <v>15</v>
+      </c>
+      <c r="X298">
+        <v>0</v>
+      </c>
+      <c r="Y298">
+        <v>2.3099251860175208E-4</v>
+      </c>
+      <c r="Z298">
+        <v>50.022296676015927</v>
+      </c>
+      <c r="AA298">
+        <v>43.733333333333334</v>
+      </c>
+      <c r="AB298">
+        <v>5.6521306295224978</v>
+      </c>
+    </row>
+    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E299">
+        <v>0.6</v>
+      </c>
+      <c r="F299">
+        <v>0.3</v>
+      </c>
+      <c r="G299">
+        <v>0.1</v>
+      </c>
+      <c r="H299">
+        <v>0.6</v>
+      </c>
+      <c r="I299">
+        <v>0.4</v>
+      </c>
+      <c r="J299">
+        <v>5</v>
+      </c>
+      <c r="K299">
+        <v>18</v>
+      </c>
+      <c r="L299" t="s">
+        <v>40</v>
+      </c>
+      <c r="O299">
+        <v>20</v>
+      </c>
+      <c r="P299">
+        <v>7</v>
+      </c>
+      <c r="Q299">
+        <v>11</v>
+      </c>
+      <c r="R299">
+        <v>5</v>
+      </c>
+      <c r="S299">
+        <v>0</v>
+      </c>
+      <c r="V299">
+        <v>15</v>
+      </c>
+      <c r="X299" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Y299" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Z299">
+        <v>50.440528969967666</v>
+      </c>
+    </row>
+    <row r="300" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>-0.5</v>
+      </c>
+      <c r="B300">
+        <v>0.5</v>
+      </c>
+      <c r="C300">
+        <v>0</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300">
+        <v>0.6</v>
+      </c>
+      <c r="F300">
+        <v>0.3</v>
+      </c>
+      <c r="G300">
+        <v>0.1</v>
+      </c>
+      <c r="H300">
+        <v>0.6</v>
+      </c>
+      <c r="I300">
+        <v>0.4</v>
+      </c>
+      <c r="J300">
+        <v>5</v>
+      </c>
+      <c r="K300">
+        <v>18</v>
+      </c>
+      <c r="L300" t="s">
+        <v>42</v>
+      </c>
+      <c r="M300" t="s">
+        <v>34</v>
+      </c>
+      <c r="N300">
+        <v>1</v>
+      </c>
+      <c r="O300">
+        <v>20</v>
+      </c>
+      <c r="P300">
+        <v>7</v>
+      </c>
+      <c r="Q300">
+        <v>11</v>
+      </c>
+      <c r="R300">
+        <v>5</v>
+      </c>
+      <c r="S300">
+        <v>2</v>
+      </c>
+      <c r="V300">
+        <v>15</v>
+      </c>
+      <c r="X300">
+        <v>0</v>
+      </c>
+      <c r="Y300">
+        <v>4.2678979730564816E-4</v>
+      </c>
+      <c r="Z300">
+        <v>50.212329731731437</v>
+      </c>
+      <c r="AA300">
+        <v>30.2</v>
+      </c>
+      <c r="AB300">
+        <v>8.1085051052462749</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="E301" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G301" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H301" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I301" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J301" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K301" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L301" t="s">
+        <v>42</v>
+      </c>
+      <c r="M301" t="s">
+        <v>34</v>
+      </c>
+      <c r="N301" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O301" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P301" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q301" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R301" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S301" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V301" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="X301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y301" t="n">
+        <v>5.087203864572238E-4</v>
+      </c>
+      <c r="Z301" t="n">
+        <v>50.23998260196259</v>
+      </c>
+      <c r="AA301" t="n">
+        <v>29.733333333333334</v>
+      </c>
+      <c r="AB301" t="n">
+        <v>8.333657211839336</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AB297"/>
@@ -27283,7 +27552,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA297"/>
+  <dimension ref="A1:AA300"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="X296" sqref="X11:X296"/>
@@ -27297,7 +27566,7 @@
     <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" hidden="true" style="1" width="0.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" hidden="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="0.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" hidden="true" width="11.140625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" hidden="true" width="13.0" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
@@ -48463,7 +48732,7 @@
         <v>548.56799999999998</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>-0.79999999999999993</v>
       </c>
@@ -48537,7 +48806,7 @@
         <v>548.56799999999998</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>-0.79999999999999993</v>
       </c>
@@ -48611,7 +48880,7 @@
         <v>551.88900000000001</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>-0.79999999999999993</v>
       </c>
@@ -48685,7 +48954,7 @@
         <v>548.56799999999998</v>
       </c>
     </row>
-    <row r="292" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>-0.79999999999999993</v>
       </c>
@@ -48759,7 +49028,7 @@
         <v>547.98099999999999</v>
       </c>
     </row>
-    <row r="293" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>-0.89999999999999991</v>
       </c>
@@ -48833,7 +49102,7 @@
         <v>551.88900000000001</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>-0.89999999999999991</v>
       </c>
@@ -48907,7 +49176,7 @@
         <v>548.56799999999998</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>-0.89999999999999991</v>
       </c>
@@ -48981,7 +49250,7 @@
         <v>547.98099999999999</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>-0.99999999999999989</v>
       </c>
@@ -49055,39 +49324,39 @@
         <v>551.88900000000001</v>
       </c>
     </row>
-    <row r="297">
-      <c r="A297" t="n">
-        <v>-0.0</v>
-      </c>
-      <c r="B297" t="n">
+    <row r="297" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>0</v>
+      </c>
+      <c r="B297">
         <v>0.7</v>
       </c>
-      <c r="C297" t="n">
+      <c r="C297">
         <v>-0.2</v>
       </c>
-      <c r="D297" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E297" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F297" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="G297" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H297" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I297" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J297" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="K297" t="n">
-        <v>18.0</v>
+      <c r="D297">
+        <v>0.1</v>
+      </c>
+      <c r="E297">
+        <v>0.6</v>
+      </c>
+      <c r="F297">
+        <v>0.3</v>
+      </c>
+      <c r="G297">
+        <v>0.1</v>
+      </c>
+      <c r="H297">
+        <v>0.6</v>
+      </c>
+      <c r="I297">
+        <v>0.4</v>
+      </c>
+      <c r="J297">
+        <v>5</v>
+      </c>
+      <c r="K297">
+        <v>18</v>
       </c>
       <c r="L297" t="s">
         <v>37</v>
@@ -49095,38 +49364,251 @@
       <c r="M297" t="s">
         <v>34</v>
       </c>
-      <c r="N297" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="O297" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="P297" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="R297" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="S297" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="T297" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U297" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="W297" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="X297" t="n">
-        <v>1.854</v>
-      </c>
-      <c r="Y297" t="n">
+      <c r="N297">
+        <v>1</v>
+      </c>
+      <c r="O297">
+        <v>20</v>
+      </c>
+      <c r="P297">
+        <v>7</v>
+      </c>
+      <c r="R297">
+        <v>5</v>
+      </c>
+      <c r="S297">
+        <v>1</v>
+      </c>
+      <c r="T297">
+        <v>3</v>
+      </c>
+      <c r="U297">
+        <v>3</v>
+      </c>
+      <c r="W297">
+        <v>5</v>
+      </c>
+      <c r="X297">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="Y297">
         <v>1.901</v>
       </c>
-      <c r="Z297" t="n">
-        <v>544.909</v>
+      <c r="Z297">
+        <v>544.90899999999999</v>
+      </c>
+    </row>
+    <row r="298" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>0</v>
+      </c>
+      <c r="B298">
+        <v>0.7</v>
+      </c>
+      <c r="C298">
+        <v>-0.2</v>
+      </c>
+      <c r="D298">
+        <v>0.1</v>
+      </c>
+      <c r="E298">
+        <v>0.6</v>
+      </c>
+      <c r="F298">
+        <v>0.3</v>
+      </c>
+      <c r="G298">
+        <v>0.1</v>
+      </c>
+      <c r="H298">
+        <v>0.6</v>
+      </c>
+      <c r="I298">
+        <v>0.4</v>
+      </c>
+      <c r="L298" t="s">
+        <v>33</v>
+      </c>
+      <c r="M298" t="s">
+        <v>34</v>
+      </c>
+      <c r="N298">
+        <v>1</v>
+      </c>
+      <c r="O298">
+        <v>20</v>
+      </c>
+      <c r="P298">
+        <v>7</v>
+      </c>
+      <c r="R298">
+        <v>5</v>
+      </c>
+      <c r="S298">
+        <v>2</v>
+      </c>
+      <c r="T298">
+        <v>3</v>
+      </c>
+      <c r="W298">
+        <v>5</v>
+      </c>
+      <c r="X298">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="Y298">
+        <v>0.45</v>
+      </c>
+      <c r="Z298">
+        <v>533.596</v>
+      </c>
+    </row>
+    <row r="299" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>0</v>
+      </c>
+      <c r="B299">
+        <v>0.7</v>
+      </c>
+      <c r="C299">
+        <v>-0.2</v>
+      </c>
+      <c r="D299">
+        <v>0.1</v>
+      </c>
+      <c r="E299">
+        <v>0.6</v>
+      </c>
+      <c r="F299">
+        <v>0.3</v>
+      </c>
+      <c r="G299">
+        <v>0.1</v>
+      </c>
+      <c r="H299">
+        <v>0.6</v>
+      </c>
+      <c r="I299">
+        <v>0.4</v>
+      </c>
+      <c r="J299">
+        <v>5</v>
+      </c>
+      <c r="K299">
+        <v>18</v>
+      </c>
+      <c r="L299" t="s">
+        <v>37</v>
+      </c>
+      <c r="M299" t="s">
+        <v>34</v>
+      </c>
+      <c r="N299">
+        <v>1</v>
+      </c>
+      <c r="O299">
+        <v>20</v>
+      </c>
+      <c r="P299">
+        <v>7</v>
+      </c>
+      <c r="R299">
+        <v>5</v>
+      </c>
+      <c r="S299">
+        <v>2</v>
+      </c>
+      <c r="T299">
+        <v>3</v>
+      </c>
+      <c r="U299">
+        <v>3</v>
+      </c>
+      <c r="W299">
+        <v>5</v>
+      </c>
+      <c r="X299">
+        <v>3.9470000000000001</v>
+      </c>
+      <c r="Y299">
+        <v>4.016</v>
+      </c>
+      <c r="Z299">
+        <v>533.596</v>
+      </c>
+    </row>
+    <row r="300" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>0</v>
+      </c>
+      <c r="B300">
+        <v>0.7</v>
+      </c>
+      <c r="C300">
+        <v>-0.2</v>
+      </c>
+      <c r="D300">
+        <v>0.1</v>
+      </c>
+      <c r="E300">
+        <v>0.6</v>
+      </c>
+      <c r="F300">
+        <v>0.3</v>
+      </c>
+      <c r="G300">
+        <v>0.1</v>
+      </c>
+      <c r="H300">
+        <v>0.6</v>
+      </c>
+      <c r="I300">
+        <v>0.4</v>
+      </c>
+      <c r="J300">
+        <v>5</v>
+      </c>
+      <c r="K300">
+        <v>18</v>
+      </c>
+      <c r="L300" t="s">
+        <v>37</v>
+      </c>
+      <c r="M300" t="s">
+        <v>34</v>
+      </c>
+      <c r="N300">
+        <v>1</v>
+      </c>
+      <c r="O300">
+        <v>20</v>
+      </c>
+      <c r="P300">
+        <v>7</v>
+      </c>
+      <c r="R300">
+        <v>5</v>
+      </c>
+      <c r="S300">
+        <v>2</v>
+      </c>
+      <c r="T300">
+        <v>3</v>
+      </c>
+      <c r="U300">
+        <v>3</v>
+      </c>
+      <c r="W300">
+        <v>5</v>
+      </c>
+      <c r="X300">
+        <v>3.73</v>
+      </c>
+      <c r="Y300">
+        <v>3.8079999999999998</v>
+      </c>
+      <c r="Z300">
+        <v>533.596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Legger til clustering på heuristikk
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="44">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -2260,7 +2260,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD301"/>
+  <dimension ref="A1:AD302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
       <selection activeCell="A301" sqref="A301"/>
@@ -27486,6 +27486,71 @@
       </c>
       <c r="AB301" t="n">
         <v>8.333657211839336</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="E302" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G302" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H302" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I302" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J302" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K302" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L302" t="s">
+        <v>42</v>
+      </c>
+      <c r="M302" t="s">
+        <v>34</v>
+      </c>
+      <c r="N302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O302" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P302" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q302" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R302" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S302" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V302" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="X302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y302" t="n">
+        <v>3.076598751774873E-4</v>
+      </c>
+      <c r="Z302" t="n">
+        <v>50.23705930469656</v>
+      </c>
+      <c r="AA302" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="AB302" t="n">
+        <v>8.409905362209615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Klar for nattesting Marte
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\masteroppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="13215"/>
+    <workbookView windowHeight="13215" windowWidth="28215" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation" sheetId="1" r:id="rId1"/>
-    <sheet name="One route" sheetId="3" r:id="rId2"/>
+    <sheet name="Simulation" r:id="rId1" sheetId="1"/>
+    <sheet name="One route" r:id="rId2" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'One route'!$A$3:$AH$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Simulation!$A$3:$AO$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'One route'!$A$3:$AH$3</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Simulation!$A$3:$AO$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="52">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -249,97 +249,97 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -356,10 +356,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -394,7 +394,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -429,7 +429,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -523,21 +523,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -554,7 +554,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -606,63 +606,63 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" style="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.5703125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="14.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.140625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.42578125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.42578125" style="7" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="17.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="7.85546875" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="9" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="9" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="16.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="9" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" hidden="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" width="11.42578125" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" hidden="true" width="9.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" hidden="true" width="10.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" hidden="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" hidden="true" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" hidden="true" width="11.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" hidden="true" width="14.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" hidden="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="18" customWidth="true" hidden="true" width="14.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" hidden="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" hidden="true" width="11.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="22.85546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="7" width="12.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="8" width="12.42578125" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="11" width="13.85546875" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="9" width="17.42578125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="6" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="57" r="1" s="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -721,7 +721,7 @@
       <c r="AN1" s="29"/>
       <c r="AO1" s="13"/>
     </row>
-    <row r="2" spans="1:41" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="2" s="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>0</v>
       </c>
@@ -844,7 +844,7 @@
       </c>
       <c r="AO2" s="13"/>
     </row>
-    <row r="3" spans="1:41" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48.75" r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15.75" r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>6.1500000000000013E-2</v>
       </c>
@@ -4288,6 +4288,59 @@
       </c>
       <c r="AN36">
         <v>50</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="n">
+        <v>42.051089094874875</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>50</v>
+      </c>
+      <c r="V37" t="s">
+        <v>49</v>
+      </c>
+      <c r="W37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X37" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>
@@ -4303,7 +4356,7 @@
     <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C25">
-    <cfRule type="colorScale" priority="6">
+    <cfRule priority="6" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4315,7 +4368,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="colorScale" priority="5">
+    <cfRule priority="5" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4327,7 +4380,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C32">
-    <cfRule type="colorScale" priority="4">
+    <cfRule priority="4" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4339,7 +4392,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C34">
-    <cfRule type="colorScale" priority="3">
+    <cfRule priority="3" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4351,7 +4404,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C35">
-    <cfRule type="colorScale" priority="2">
+    <cfRule priority="2" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4363,7 +4416,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 C1">
-    <cfRule type="colorScale" priority="1">
+    <cfRule priority="1" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4374,57 +4427,57 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="21" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" style="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" style="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.140625" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.7109375" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.140625" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5703125" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.7109375" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5703125" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" style="1" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.140625" style="21" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="25.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.7109375" style="21" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="14.5703125" style="21" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="9.140625" style="21" collapsed="1"/>
-    <col min="24" max="24" width="11.140625" style="21" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="14.85546875" style="21" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.5703125" style="21" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.7109375" style="21" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9" style="21" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.28515625" style="21" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.140625" style="21" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.140625" style="1" collapsed="1"/>
-    <col min="35" max="16384" width="9.140625" style="21" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="21" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="21" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="21" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" hidden="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" hidden="true" style="21" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" hidden="true" style="21" width="11.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" hidden="true" style="21" width="11.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" hidden="true" style="21" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" hidden="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" hidden="true" style="21" width="10.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" hidden="true" style="21" width="8.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" hidden="true" style="21" width="10.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" hidden="true" style="21" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" hidden="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" hidden="true" style="21" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" hidden="true" style="21" width="10.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" hidden="true" style="1" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" hidden="true" style="21" width="13.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="25.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="21" width="12.7109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="21" width="14.5703125" collapsed="true"/>
+    <col min="22" max="23" style="21" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="21" width="11.140625" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="21" width="14.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="21" width="10.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="21" width="10.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="21" width="9.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="21" width="11.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="21" width="12.140625" collapsed="true"/>
+    <col min="34" max="34" style="1" width="9.140625" collapsed="true"/>
+    <col min="35" max="16384" style="21" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="32.25" r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>25</v>
       </c>
@@ -4475,7 +4528,7 @@
       <c r="AF1" s="29"/>
       <c r="AG1" s="29"/>
     </row>
-    <row r="2" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="16.5" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>0</v>
       </c>
@@ -4576,7 +4629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="57.75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>26</v>
       </c>
@@ -6417,7 +6470,7 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:R1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resultater fra heuristikk 1, branching constant
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Average number of times vehicle route generated</t>
   </si>
   <si>
-    <t>Average time to generating new routes</t>
-  </si>
-  <si>
     <t>Objective value</t>
   </si>
   <si>
@@ -174,6 +171,18 @@
   </si>
   <si>
     <t>T-test</t>
+  </si>
+  <si>
+    <t>EVERY_VEHICLE_ARRIVAL</t>
+  </si>
+  <si>
+    <t>Computational time Xpress (sek)</t>
+  </si>
+  <si>
+    <t>Computational time Xpress + initialization (sec)</t>
+  </si>
+  <si>
+    <t>Average time to generating new routes (min)</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BF14" sqref="BF14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +662,8 @@
     <col min="38" max="38" width="7.85546875" customWidth="1" collapsed="1"/>
     <col min="39" max="39" width="11" customWidth="1" collapsed="1"/>
     <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="9.140625" style="1" collapsed="1"/>
+    <col min="41" max="41" width="0" style="1" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="50" width="0" hidden="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="6" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -679,12 +689,12 @@
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="29"/>
       <c r="R1" s="30"/>
       <c r="S1" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T1" s="31"/>
       <c r="U1" s="28" t="s">
@@ -702,19 +712,19 @@
       <c r="AE1" s="31"/>
       <c r="AF1" s="31"/>
       <c r="AG1" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AH1" s="27"/>
       <c r="AI1" s="27"/>
       <c r="AJ1" s="27"/>
       <c r="AK1" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AL1" s="27"/>
       <c r="AM1" s="27"/>
       <c r="AN1" s="27"/>
       <c r="AO1" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AP1" s="27"/>
       <c r="AQ1" s="27"/>
@@ -883,12 +893,12 @@
       <c r="AZ2" s="25"/>
       <c r="BA2" s="25"/>
     </row>
-    <row r="3" spans="1:53" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>28</v>
@@ -897,7 +907,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>1</v>
@@ -912,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>5</v>
@@ -930,13 +940,13 @@
         <v>9</v>
       </c>
       <c r="P3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>10</v>
@@ -978,31 +988,31 @@
         <v>22</v>
       </c>
       <c r="AF3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AG3" s="13" t="s">
+      <c r="AH3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" s="14" t="s">
+      <c r="AI3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AI3" s="15" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AJ3" s="16" t="s">
+      <c r="AK3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL3" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL3" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="AM3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="AN3" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AO3" s="1">
         <v>1</v>
@@ -1035,6 +1045,1226 @@
         <v>10</v>
       </c>
       <c r="AY3" s="20"/>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>0.11112485827213767</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.12301523528780882</v>
+      </c>
+      <c r="C4" s="9">
+        <v>49.34002731186736</v>
+      </c>
+      <c r="D4">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E4">
+        <v>6.910226522478359</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.7</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.3</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>0.3</v>
+      </c>
+      <c r="M4">
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <v>0.6</v>
+      </c>
+      <c r="O4">
+        <v>0.4</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <v>18</v>
+      </c>
+      <c r="U4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>20</v>
+      </c>
+      <c r="Y4">
+        <v>7</v>
+      </c>
+      <c r="Z4">
+        <v>11</v>
+      </c>
+      <c r="AA4">
+        <v>5</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>10</v>
+      </c>
+      <c r="AF4">
+        <v>5</v>
+      </c>
+      <c r="AG4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>42.155963302752291</v>
+      </c>
+      <c r="AP4">
+        <v>49.514629291304232</v>
+      </c>
+      <c r="AQ4">
+        <v>50.34209383145091</v>
+      </c>
+      <c r="AR4">
+        <v>49.763161738622372</v>
+      </c>
+      <c r="AS4">
+        <v>49.563202294021544</v>
+      </c>
+      <c r="AT4">
+        <v>49.222162653551202</v>
+      </c>
+      <c r="AU4">
+        <v>50.341862350703217</v>
+      </c>
+      <c r="AV4">
+        <v>50.478233086795733</v>
+      </c>
+      <c r="AW4">
+        <v>50.441907929548726</v>
+      </c>
+      <c r="AX4">
+        <v>51.577056639923356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>0.13246272979157742</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.15631802698708222</v>
+      </c>
+      <c r="C5" s="9">
+        <v>49.265066753665153</v>
+      </c>
+      <c r="D5">
+        <v>47.1</v>
+      </c>
+      <c r="E5">
+        <v>5.1626436345377904</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.7</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.3</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5">
+        <v>0.6</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="M5">
+        <v>0.1</v>
+      </c>
+      <c r="N5">
+        <v>0.6</v>
+      </c>
+      <c r="O5">
+        <v>0.4</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>18</v>
+      </c>
+      <c r="U5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>20</v>
+      </c>
+      <c r="Y5">
+        <v>7</v>
+      </c>
+      <c r="Z5">
+        <v>11</v>
+      </c>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>10</v>
+      </c>
+      <c r="AE5">
+        <v>10</v>
+      </c>
+      <c r="AF5">
+        <v>5</v>
+      </c>
+      <c r="AG5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>42.045871559633028</v>
+      </c>
+      <c r="AP5">
+        <v>49.280124342159084</v>
+      </c>
+      <c r="AQ5">
+        <v>50.262452939472922</v>
+      </c>
+      <c r="AR5">
+        <v>49.70543023878583</v>
+      </c>
+      <c r="AS5">
+        <v>49.507074344525584</v>
+      </c>
+      <c r="AT5">
+        <v>49.162024195240207</v>
+      </c>
+      <c r="AU5">
+        <v>50.298593569713411</v>
+      </c>
+      <c r="AV5">
+        <v>50.433026974113545</v>
+      </c>
+      <c r="AW5">
+        <v>50.418928112480152</v>
+      </c>
+      <c r="AX5">
+        <v>51.537141260527683</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>0.21875392473299132</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.30030807117427744</v>
+      </c>
+      <c r="C6" s="9">
+        <v>49.281924974912741</v>
+      </c>
+      <c r="D6">
+        <v>45.9</v>
+      </c>
+      <c r="E6">
+        <v>5.2937821570624539</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.3</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>0.6</v>
+      </c>
+      <c r="L6">
+        <v>0.3</v>
+      </c>
+      <c r="M6">
+        <v>0.1</v>
+      </c>
+      <c r="N6">
+        <v>0.6</v>
+      </c>
+      <c r="O6">
+        <v>0.4</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>18</v>
+      </c>
+      <c r="U6" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>20</v>
+      </c>
+      <c r="Y6">
+        <v>7</v>
+      </c>
+      <c r="Z6">
+        <v>11</v>
+      </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
+        <v>20</v>
+      </c>
+      <c r="AE6">
+        <v>10</v>
+      </c>
+      <c r="AF6">
+        <v>5</v>
+      </c>
+      <c r="AG6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>42.137614678899084</v>
+      </c>
+      <c r="AP6">
+        <v>49.35374798898372</v>
+      </c>
+      <c r="AQ6">
+        <v>50.19638719953663</v>
+      </c>
+      <c r="AR6">
+        <v>49.737426009779576</v>
+      </c>
+      <c r="AS6">
+        <v>49.538750514043102</v>
+      </c>
+      <c r="AT6">
+        <v>49.174145124822267</v>
+      </c>
+      <c r="AU6">
+        <v>50.305999937630588</v>
+      </c>
+      <c r="AV6">
+        <v>50.433706765281705</v>
+      </c>
+      <c r="AW6">
+        <v>50.399274321566253</v>
+      </c>
+      <c r="AX6">
+        <v>51.542197208584476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>0.57990543577198772</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.81702272896908601</v>
+      </c>
+      <c r="C7" s="9">
+        <v>49.267974428199963</v>
+      </c>
+      <c r="D7">
+        <v>47.6</v>
+      </c>
+      <c r="E7">
+        <v>5.1352392923320185</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.7</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.3</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>0.6</v>
+      </c>
+      <c r="L7">
+        <v>0.3</v>
+      </c>
+      <c r="M7">
+        <v>0.1</v>
+      </c>
+      <c r="N7">
+        <v>0.6</v>
+      </c>
+      <c r="O7">
+        <v>0.4</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>18</v>
+      </c>
+      <c r="U7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V7" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>20</v>
+      </c>
+      <c r="Y7">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>11</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>30</v>
+      </c>
+      <c r="AE7">
+        <v>10</v>
+      </c>
+      <c r="AF7">
+        <v>5</v>
+      </c>
+      <c r="AG7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>41.960244648318039</v>
+      </c>
+      <c r="AP7">
+        <v>49.267853734354979</v>
+      </c>
+      <c r="AQ7">
+        <v>50.267883000289601</v>
+      </c>
+      <c r="AR7">
+        <v>49.726992606194656</v>
+      </c>
+      <c r="AS7">
+        <v>49.547642070398894</v>
+      </c>
+      <c r="AT7">
+        <v>49.197454604787765</v>
+      </c>
+      <c r="AU7">
+        <v>50.305610128792843</v>
+      </c>
+      <c r="AV7">
+        <v>50.435746138786165</v>
+      </c>
+      <c r="AW7">
+        <v>50.426789628845711</v>
+      </c>
+      <c r="AX7">
+        <v>51.543527721230987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>1.8904670796001732</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2.5892789131377874</v>
+      </c>
+      <c r="C8" s="9">
+        <v>49.282103714474154</v>
+      </c>
+      <c r="D8">
+        <v>50.9</v>
+      </c>
+      <c r="E8">
+        <v>4.7765860085833776</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.7</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.3</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>0.6</v>
+      </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+      <c r="M8">
+        <v>0.1</v>
+      </c>
+      <c r="N8">
+        <v>0.6</v>
+      </c>
+      <c r="O8">
+        <v>0.4</v>
+      </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
+      <c r="T8">
+        <v>18</v>
+      </c>
+      <c r="U8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>20</v>
+      </c>
+      <c r="Y8">
+        <v>7</v>
+      </c>
+      <c r="Z8">
+        <v>11</v>
+      </c>
+      <c r="AA8">
+        <v>5</v>
+      </c>
+      <c r="AB8">
+        <v>2</v>
+      </c>
+      <c r="AC8">
+        <v>40</v>
+      </c>
+      <c r="AE8">
+        <v>10</v>
+      </c>
+      <c r="AF8">
+        <v>5</v>
+      </c>
+      <c r="AG8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>42.018348623853214</v>
+      </c>
+      <c r="AP8">
+        <v>49.325116570774142</v>
+      </c>
+      <c r="AQ8">
+        <v>50.274218071242395</v>
+      </c>
+      <c r="AR8">
+        <v>49.734643768823602</v>
+      </c>
+      <c r="AS8">
+        <v>49.528191790870594</v>
+      </c>
+      <c r="AT8">
+        <v>49.198853173585697</v>
+      </c>
+      <c r="AU8">
+        <v>50.306779555306079</v>
+      </c>
+      <c r="AV8">
+        <v>50.45885903850337</v>
+      </c>
+      <c r="AW8">
+        <v>50.425580164789473</v>
+      </c>
+      <c r="AX8">
+        <v>51.55044638699291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>1.5575755344315407</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.5697160593636135</v>
+      </c>
+      <c r="C9" s="9">
+        <v>49.412501410982458</v>
+      </c>
+      <c r="D9">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E9">
+        <v>6.8963638131344283</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.7</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.3</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>0.6</v>
+      </c>
+      <c r="L9">
+        <v>0.3</v>
+      </c>
+      <c r="M9">
+        <v>0.1</v>
+      </c>
+      <c r="N9">
+        <v>0.6</v>
+      </c>
+      <c r="O9">
+        <v>0.4</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>18</v>
+      </c>
+      <c r="U9" t="s">
+        <v>45</v>
+      </c>
+      <c r="V9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>20</v>
+      </c>
+      <c r="Y9">
+        <v>7</v>
+      </c>
+      <c r="Z9">
+        <v>11</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AE9">
+        <v>10</v>
+      </c>
+      <c r="AF9">
+        <v>5</v>
+      </c>
+      <c r="AG9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>42.581039755351682</v>
+      </c>
+      <c r="AP9">
+        <v>49.60325034766722</v>
+      </c>
+      <c r="AQ9">
+        <v>50.345713871995365</v>
+      </c>
+      <c r="AR9">
+        <v>49.859149051603616</v>
+      </c>
+      <c r="AS9">
+        <v>49.5954341858113</v>
+      </c>
+      <c r="AT9">
+        <v>49.240810237523604</v>
+      </c>
+      <c r="AU9">
+        <v>50.355115851186582</v>
+      </c>
+      <c r="AV9">
+        <v>50.49488797041549</v>
+      </c>
+      <c r="AW9">
+        <v>50.46670194270164</v>
+      </c>
+      <c r="AX9">
+        <v>51.582910895568055</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>2.0472493677323937</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2.058478510987491</v>
+      </c>
+      <c r="C10" s="9">
+        <v>49.393507691030869</v>
+      </c>
+      <c r="D10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E10">
+        <v>6.7687360612478589</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.7</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.3</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0.6</v>
+      </c>
+      <c r="L10">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <v>0.1</v>
+      </c>
+      <c r="N10">
+        <v>0.6</v>
+      </c>
+      <c r="O10">
+        <v>0.4</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>18</v>
+      </c>
+      <c r="U10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10" t="s">
+        <v>49</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>20</v>
+      </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
+        <v>10</v>
+      </c>
+      <c r="AF10">
+        <v>5</v>
+      </c>
+      <c r="AG10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>42.525993883792054</v>
+      </c>
+      <c r="AP10">
+        <v>49.533716903443953</v>
+      </c>
+      <c r="AQ10">
+        <v>50.354763973356498</v>
+      </c>
+      <c r="AR10">
+        <v>49.814633196307966</v>
+      </c>
+      <c r="AS10">
+        <v>49.603770019894853</v>
+      </c>
+      <c r="AT10">
+        <v>49.241276427122912</v>
+      </c>
+      <c r="AU10">
+        <v>50.352387189322357</v>
+      </c>
+      <c r="AV10">
+        <v>50.479592669132046</v>
+      </c>
+      <c r="AW10">
+        <v>50.4518860080127</v>
+      </c>
+      <c r="AX10">
+        <v>51.577056639923356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>2.5837133164051429</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2.5947944362514175</v>
+      </c>
+      <c r="C11" s="9">
+        <v>49.370781909434449</v>
+      </c>
+      <c r="D11">
+        <v>35.4</v>
+      </c>
+      <c r="E11">
+        <v>6.9024514891936963</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.7</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.3</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>0.6</v>
+      </c>
+      <c r="L11">
+        <v>0.3</v>
+      </c>
+      <c r="M11">
+        <v>0.1</v>
+      </c>
+      <c r="N11">
+        <v>0.6</v>
+      </c>
+      <c r="O11">
+        <v>0.4</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11">
+        <v>18</v>
+      </c>
+      <c r="U11" t="s">
+        <v>45</v>
+      </c>
+      <c r="V11" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>7</v>
+      </c>
+      <c r="Z11">
+        <v>11</v>
+      </c>
+      <c r="AA11">
+        <v>5</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AE11">
+        <v>10</v>
+      </c>
+      <c r="AF11">
+        <v>5</v>
+      </c>
+      <c r="AG11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>42.296636085626908</v>
+      </c>
+      <c r="AP11">
+        <v>49.528263299975464</v>
+      </c>
+      <c r="AQ11">
+        <v>50.38734433825659</v>
+      </c>
+      <c r="AR11">
+        <v>49.777768503641255</v>
+      </c>
+      <c r="AS11">
+        <v>49.599324241716957</v>
+      </c>
+      <c r="AT11">
+        <v>49.245472133516699</v>
+      </c>
+      <c r="AU11">
+        <v>50.340303115352235</v>
+      </c>
+      <c r="AV11">
+        <v>50.491149118990641</v>
+      </c>
+      <c r="AW11">
+        <v>50.452793106054884</v>
+      </c>
+      <c r="AX11">
+        <v>51.588765151212769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>3.7967190429599631</v>
+      </c>
+      <c r="B12" s="9">
+        <v>3.809955058479531</v>
+      </c>
+      <c r="C12" s="9">
+        <v>49.358437887105922</v>
+      </c>
+      <c r="D12">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E12">
+        <v>6.4838473976383257</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.7</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.3</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>0.6</v>
+      </c>
+      <c r="L12">
+        <v>0.3</v>
+      </c>
+      <c r="M12">
+        <v>0.1</v>
+      </c>
+      <c r="N12">
+        <v>0.6</v>
+      </c>
+      <c r="O12">
+        <v>0.4</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>18</v>
+      </c>
+      <c r="U12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>20</v>
+      </c>
+      <c r="Y12">
+        <v>7</v>
+      </c>
+      <c r="Z12">
+        <v>11</v>
+      </c>
+      <c r="AA12">
+        <v>5</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
+      </c>
+      <c r="AC12">
+        <v>6</v>
+      </c>
+      <c r="AE12">
+        <v>10</v>
+      </c>
+      <c r="AF12">
+        <v>5</v>
+      </c>
+      <c r="AG12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>42.311926605504588</v>
+      </c>
+      <c r="AP12">
+        <v>49.456003054017941</v>
+      </c>
+      <c r="AQ12">
+        <v>50.341188821314795</v>
+      </c>
+      <c r="AR12">
+        <v>49.797244190333103</v>
+      </c>
+      <c r="AS12">
+        <v>49.586542629455508</v>
+      </c>
+      <c r="AT12">
+        <v>49.225892170345681</v>
+      </c>
+      <c r="AU12">
+        <v>50.362912027941498</v>
+      </c>
+      <c r="AV12">
+        <v>50.469735697193819</v>
+      </c>
+      <c r="AW12">
+        <v>50.45853806032202</v>
+      </c>
+      <c r="AX12">
+        <v>51.574395614630319</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>6.57998553715385</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6.5928842834016548</v>
+      </c>
+      <c r="C13" s="9">
+        <v>49.326936068780633</v>
+      </c>
+      <c r="D13">
+        <v>40.5</v>
+      </c>
+      <c r="E13">
+        <v>6.0928815311181257</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.7</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.3</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>0.6</v>
+      </c>
+      <c r="L13">
+        <v>0.3</v>
+      </c>
+      <c r="M13">
+        <v>0.1</v>
+      </c>
+      <c r="N13">
+        <v>0.6</v>
+      </c>
+      <c r="O13">
+        <v>0.4</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>18</v>
+      </c>
+      <c r="U13" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" t="s">
+        <v>49</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>20</v>
+      </c>
+      <c r="Y13">
+        <v>7</v>
+      </c>
+      <c r="Z13">
+        <v>11</v>
+      </c>
+      <c r="AA13">
+        <v>5</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
+      </c>
+      <c r="AC13">
+        <v>7</v>
+      </c>
+      <c r="AE13">
+        <v>10</v>
+      </c>
+      <c r="AF13">
+        <v>5</v>
+      </c>
+      <c r="AG13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>42.217125382262999</v>
+      </c>
+      <c r="AP13">
+        <v>49.468273661822046</v>
+      </c>
+      <c r="AQ13">
+        <v>50.325803649000868</v>
+      </c>
+      <c r="AR13">
+        <v>49.77985518435824</v>
+      </c>
+      <c r="AS13">
+        <v>49.517077345425847</v>
+      </c>
+      <c r="AT13">
+        <v>49.205846017575347</v>
+      </c>
+      <c r="AU13">
+        <v>50.319253438113954</v>
+      </c>
+      <c r="AV13">
+        <v>50.457159560582987</v>
+      </c>
+      <c r="AW13">
+        <v>50.416811550381738</v>
+      </c>
+      <c r="AX13">
+        <v>51.562154898282309</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:AN3"/>
@@ -1049,7 +2279,19 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:AF1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C1048576 C1">
+  <conditionalFormatting sqref="C3:C7 C1 C9:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1132,12 +2374,12 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R1" s="29"/>
       <c r="S1" s="28" t="s">
@@ -1151,12 +2393,12 @@
       <c r="Y1" s="29"/>
       <c r="Z1" s="29"/>
       <c r="AA1" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB1" s="27"/>
       <c r="AC1" s="27"/>
       <c r="AD1" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE1" s="27"/>
       <c r="AF1" s="27"/>
@@ -1271,7 +2513,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>1</v>
@@ -1286,7 +2528,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
@@ -1304,13 +2546,13 @@
         <v>9</v>
       </c>
       <c r="N3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>10</v>
@@ -1337,31 +2579,31 @@
         <v>20</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="AB3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AD3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="21" t="s">
-        <v>39</v>
       </c>
       <c r="AF3" s="21" t="s">
         <v>20</v>
       </c>
       <c r="AG3" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1411,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="S4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T4">
         <v>1</v>
@@ -1490,7 +2732,7 @@
         <v>18</v>
       </c>
       <c r="S5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T5">
         <v>1</v>
@@ -1572,7 +2814,7 @@
         <v>18</v>
       </c>
       <c r="S6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -1651,7 +2893,7 @@
         <v>18</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1734,7 +2976,7 @@
         <v>18</v>
       </c>
       <c r="S8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T8">
         <v>1</v>
@@ -1814,7 +3056,7 @@
         <v>18</v>
       </c>
       <c r="S9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T9">
         <v>1</v>
@@ -1888,7 +3130,7 @@
         <v>18</v>
       </c>
       <c r="S10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T10">
         <v>1</v>
@@ -1971,7 +3213,7 @@
         <v>18</v>
       </c>
       <c r="S11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T11">
         <v>1</v>
@@ -2051,7 +3293,7 @@
         <v>18</v>
       </c>
       <c r="S12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T12">
         <v>1</v>
@@ -2134,7 +3376,7 @@
         <v>18</v>
       </c>
       <c r="S13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T13">
         <v>1</v>
@@ -2223,7 +3465,7 @@
         <v>18</v>
       </c>
       <c r="S14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T14">
         <v>1</v>
@@ -2303,7 +3545,7 @@
         <v>18</v>
       </c>
       <c r="S15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T15">
         <v>1</v>
@@ -2386,7 +3628,7 @@
         <v>18</v>
       </c>
       <c r="S16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T16">
         <v>1</v>
@@ -2484,7 +3726,7 @@
         <v>18</v>
       </c>
       <c r="S17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T17">
         <v>1</v>
@@ -2573,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="S18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T18">
         <v>1</v>
@@ -2662,7 +3904,7 @@
         <v>18</v>
       </c>
       <c r="S19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T19">
         <v>1</v>
@@ -2751,7 +3993,7 @@
         <v>18</v>
       </c>
       <c r="S20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T20">
         <v>1</v>
@@ -2825,7 +4067,7 @@
         <v>18</v>
       </c>
       <c r="S21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T21">
         <v>1</v>
@@ -2908,7 +4150,7 @@
         <v>18</v>
       </c>
       <c r="S22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T22">
         <v>1</v>
@@ -2991,7 +4233,7 @@
         <v>18</v>
       </c>
       <c r="S23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T23">
         <v>1</v>
@@ -3065,7 +4307,7 @@
         <v>18</v>
       </c>
       <c r="S24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T24">
         <v>1</v>

</xml_diff>

<commit_message>
Results branching constant V3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="54">
   <si>
     <t>Criticality score, weights</t>
   </si>
@@ -14772,7 +14772,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI108"/>
+  <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="T53" sqref="T53"/>
@@ -23294,6 +23294,2470 @@
         <v>17.0</v>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>0.201</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.271</v>
+      </c>
+      <c r="C109" t="n">
+        <v>56.3418</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H109" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I109" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K109" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L109" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M109" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R109" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S109" t="s">
+        <v>47</v>
+      </c>
+      <c r="T109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U109" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W109" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X109" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z109" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA109" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD109" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH109" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="C110" t="n">
+        <v>27.1529</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H110" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L110" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M110" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R110" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S110" t="s">
+        <v>47</v>
+      </c>
+      <c r="T110" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U110" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V110" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W110" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X110" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z110" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA110" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD110" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH110" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="C111" t="n">
+        <v>217.517</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H111" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L111" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M111" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R111" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S111" t="s">
+        <v>47</v>
+      </c>
+      <c r="T111" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U111" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V111" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W111" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X111" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z111" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA111" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD111" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH111" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="C112" t="n">
+        <v>168.943</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H112" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L112" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M112" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R112" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S112" t="s">
+        <v>47</v>
+      </c>
+      <c r="T112" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U112" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V112" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W112" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X112" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z112" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA112" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD112" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH112" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="C113" t="n">
+        <v>395.854</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H113" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I113" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K113" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L113" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M113" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R113" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S113" t="s">
+        <v>47</v>
+      </c>
+      <c r="T113" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U113" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V113" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W113" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X113" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z113" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA113" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD113" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH113" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.192</v>
+      </c>
+      <c r="C114" t="n">
+        <v>243.739</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H114" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L114" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M114" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R114" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S114" t="s">
+        <v>47</v>
+      </c>
+      <c r="T114" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U114" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V114" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W114" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X114" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z114" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA114" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD114" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH114" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="C115" t="n">
+        <v>540.204</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H115" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L115" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M115" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q115" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R115" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S115" t="s">
+        <v>47</v>
+      </c>
+      <c r="T115" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U115" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V115" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W115" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X115" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z115" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA115" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD115" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH115" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="C116" t="n">
+        <v>372.207</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H116" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L116" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M116" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R116" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S116" t="s">
+        <v>47</v>
+      </c>
+      <c r="T116" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U116" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V116" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W116" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X116" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z116" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA116" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD116" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH116" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="C117" t="n">
+        <v>56.3418</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H117" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M117" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q117" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R117" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S117" t="s">
+        <v>47</v>
+      </c>
+      <c r="T117" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U117" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V117" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W117" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X117" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z117" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA117" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD117" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH117" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="C118" t="n">
+        <v>27.1529</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H118" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R118" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S118" t="s">
+        <v>47</v>
+      </c>
+      <c r="T118" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U118" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V118" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W118" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X118" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z118" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA118" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD118" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH118" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="C119" t="n">
+        <v>217.517</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H119" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L119" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M119" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q119" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R119" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S119" t="s">
+        <v>47</v>
+      </c>
+      <c r="T119" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U119" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V119" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W119" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X119" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z119" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA119" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD119" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH119" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.198</v>
+      </c>
+      <c r="C120" t="n">
+        <v>167.83</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H120" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L120" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M120" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q120" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R120" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S120" t="s">
+        <v>47</v>
+      </c>
+      <c r="T120" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U120" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V120" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W120" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X120" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z120" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA120" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD120" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH120" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="C121" t="n">
+        <v>391.14</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H121" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L121" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M121" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q121" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R121" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S121" t="s">
+        <v>47</v>
+      </c>
+      <c r="T121" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U121" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V121" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W121" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X121" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z121" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA121" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD121" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH121" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="C122" t="n">
+        <v>240.106</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H122" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M122" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R122" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S122" t="s">
+        <v>47</v>
+      </c>
+      <c r="T122" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U122" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V122" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W122" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X122" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z122" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA122" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD122" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH122" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0.209</v>
+      </c>
+      <c r="C123" t="n">
+        <v>538.53</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H123" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J123" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L123" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M123" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R123" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S123" t="s">
+        <v>47</v>
+      </c>
+      <c r="T123" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U123" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V123" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W123" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X123" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z123" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA123" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD123" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH123" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="B124" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="C124" t="n">
+        <v>369.389</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H124" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J124" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L124" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M124" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R124" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S124" t="s">
+        <v>47</v>
+      </c>
+      <c r="T124" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U124" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V124" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W124" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X124" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z124" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA124" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD124" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH124" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="C125" t="n">
+        <v>56.3418</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H125" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M125" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R125" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S125" t="s">
+        <v>47</v>
+      </c>
+      <c r="T125" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U125" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V125" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W125" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X125" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z125" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA125" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD125" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH125" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="B126" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="C126" t="n">
+        <v>27.1529</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G126" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H126" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J126" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L126" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M126" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R126" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S126" t="s">
+        <v>47</v>
+      </c>
+      <c r="T126" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U126" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V126" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W126" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X126" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z126" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA126" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD126" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH126" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="B127" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="C127" t="n">
+        <v>214.738</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H127" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J127" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M127" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R127" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S127" t="s">
+        <v>47</v>
+      </c>
+      <c r="T127" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U127" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V127" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W127" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X127" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z127" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA127" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD127" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH127" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="C128" t="n">
+        <v>167.83</v>
+      </c>
+      <c r="D128" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H128" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L128" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M128" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R128" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S128" t="s">
+        <v>47</v>
+      </c>
+      <c r="T128" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U128" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V128" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W128" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X128" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z128" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA128" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD128" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH128" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="C129" t="n">
+        <v>391.14</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H129" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L129" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M129" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q129" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R129" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S129" t="s">
+        <v>47</v>
+      </c>
+      <c r="T129" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U129" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V129" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W129" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X129" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z129" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA129" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD129" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH129" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.288</v>
+      </c>
+      <c r="C130" t="n">
+        <v>240.106</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H130" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I130" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L130" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M130" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R130" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S130" t="s">
+        <v>47</v>
+      </c>
+      <c r="T130" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U130" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V130" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W130" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X130" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z130" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA130" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD130" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH130" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="C131" t="n">
+        <v>535.56</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H131" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R131" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S131" t="s">
+        <v>47</v>
+      </c>
+      <c r="T131" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U131" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V131" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W131" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X131" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z131" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA131" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD131" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH131" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="B132" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="C132" t="n">
+        <v>369.389</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H132" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R132" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S132" t="s">
+        <v>47</v>
+      </c>
+      <c r="T132" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U132" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V132" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W132" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X132" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z132" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA132" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD132" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH132" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="B133" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="C133" t="n">
+        <v>56.3418</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H133" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I133" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L133" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M133" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R133" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S133" t="s">
+        <v>47</v>
+      </c>
+      <c r="T133" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U133" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V133" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W133" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X133" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z133" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA133" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD133" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH133" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="B134" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="C134" t="n">
+        <v>27.1529</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H134" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I134" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M134" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R134" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S134" t="s">
+        <v>47</v>
+      </c>
+      <c r="T134" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U134" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V134" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W134" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X134" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z134" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA134" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD134" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH134" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="C135" t="n">
+        <v>214.738</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H135" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I135" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L135" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M135" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q135" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R135" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S135" t="s">
+        <v>47</v>
+      </c>
+      <c r="T135" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U135" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V135" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W135" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X135" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z135" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA135" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD135" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH135" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="B136" t="n">
+        <v>0.657</v>
+      </c>
+      <c r="C136" t="n">
+        <v>167.83</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H136" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I136" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q136" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R136" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S136" t="s">
+        <v>47</v>
+      </c>
+      <c r="T136" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U136" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V136" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W136" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X136" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z136" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA136" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD136" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH136" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1.214</v>
+      </c>
+      <c r="C137" t="n">
+        <v>391.14</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H137" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I137" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L137" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M137" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R137" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S137" t="s">
+        <v>47</v>
+      </c>
+      <c r="T137" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U137" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V137" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W137" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X137" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z137" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA137" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD137" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH137" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>0.622</v>
+      </c>
+      <c r="B138" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="C138" t="n">
+        <v>240.106</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G138" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H138" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I138" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K138" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L138" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M138" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R138" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S138" t="s">
+        <v>47</v>
+      </c>
+      <c r="T138" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U138" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V138" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W138" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X138" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z138" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA138" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD138" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH138" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>1.629</v>
+      </c>
+      <c r="B139" t="n">
+        <v>2.357</v>
+      </c>
+      <c r="C139" t="n">
+        <v>535.56</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H139" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R139" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S139" t="s">
+        <v>47</v>
+      </c>
+      <c r="T139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U139" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V139" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X139" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z139" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA139" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD139" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH139" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>0.804</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1.214</v>
+      </c>
+      <c r="C140" t="n">
+        <v>369.389</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H140" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L140" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R140" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S140" t="s">
+        <v>47</v>
+      </c>
+      <c r="T140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U140" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V140" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W140" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X140" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z140" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AA140" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD140" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH140" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:AH3"/>
   <mergeCells count="8">

</xml_diff>